<commit_message>
Justeringar för fler klasser och olika typer av tävlingar
</commit_message>
<xml_diff>
--- a/mallar/Protokoll 2017 lättklass lag o ind_justerad.xlsx
+++ b/mallar/Protokoll 2017 lättklass lag o ind_justerad.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Andersson\Dropbox\Voltige (1)\Protokoll 2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="muK/Rsgn0FngGE/mV/SY/MPxEFarFdZF3g0P1PGbjFCV9x5F8AG9QOlpeVa8cMCwcnfLIvLNCjpGfdHDMXsAuQ==" workbookSaltValue="s+AIShC46YCzrqNSDCe49g==" workbookSpinCount="100000" lockStructure="1"/>
@@ -20,7 +20,49 @@
     <sheet name="Lätt ind grund" sheetId="6" r:id="rId5"/>
     <sheet name="Lätt ind kür" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="armnr" localSheetId="4">'Lätt ind grund'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="5">'Lätt ind kür'!$K$7</definedName>
+    <definedName name="bord" localSheetId="1">'Lätt grund'!$K$3</definedName>
+    <definedName name="bord" localSheetId="4">'Lätt ind grund'!$L$3</definedName>
+    <definedName name="bord" localSheetId="5">'Lätt ind kür'!$K$3</definedName>
+    <definedName name="bord" localSheetId="2">'Lätt lagkür 1'!$K$3</definedName>
+    <definedName name="bord" localSheetId="3">'Lätt lagkür 2'!$L$3</definedName>
+    <definedName name="datum" localSheetId="1">'Lätt grund'!$C$4</definedName>
+    <definedName name="datum" localSheetId="4">'Lätt ind grund'!$C$4</definedName>
+    <definedName name="datum" localSheetId="5">'Lätt ind kür'!$C$4</definedName>
+    <definedName name="datum" localSheetId="2">'Lätt lagkür 1'!$C$4</definedName>
+    <definedName name="datum" localSheetId="3">'Lätt lagkür 2'!$C$4</definedName>
+    <definedName name="domare" localSheetId="1">'Lätt grund'!$B$40</definedName>
+    <definedName name="domare" localSheetId="4">'Lätt ind grund'!$C$35</definedName>
+    <definedName name="domare" localSheetId="5">'Lätt ind kür'!$B$41</definedName>
+    <definedName name="domare" localSheetId="2">'Lätt lagkür 1'!$B$44</definedName>
+    <definedName name="domare" localSheetId="3">'Lätt lagkür 2'!$B$42</definedName>
+    <definedName name="firstvaulter" localSheetId="1">'Lätt grund'!$H$7</definedName>
+    <definedName name="firstvaulter" localSheetId="2">'Lätt lagkür 1'!$H$7</definedName>
+    <definedName name="firstvaulter" localSheetId="3">'Lätt lagkür 2'!$I$7</definedName>
+    <definedName name="id" localSheetId="1">'Lätt grund'!$L$2</definedName>
+    <definedName name="id" localSheetId="4">'Lätt ind grund'!$M$1</definedName>
+    <definedName name="id" localSheetId="5">'Lätt ind kür'!$L$1</definedName>
+    <definedName name="id" localSheetId="2">'Lätt lagkür 1'!$L$3</definedName>
+    <definedName name="id" localSheetId="3">'Lätt lagkür 2'!$M$3</definedName>
+    <definedName name="klass" localSheetId="1">'Lätt grund'!$K$4</definedName>
+    <definedName name="klass" localSheetId="4">'Lätt ind grund'!$L$4</definedName>
+    <definedName name="klass" localSheetId="5">'Lätt ind kür'!$K$4</definedName>
+    <definedName name="klass" localSheetId="2">'Lätt lagkür 1'!$K$4</definedName>
+    <definedName name="klass" localSheetId="3">'Lätt lagkür 2'!$L$4</definedName>
+    <definedName name="moment" localSheetId="1">'Lätt grund'!$K$5</definedName>
+    <definedName name="moment" localSheetId="4">'Lätt ind grund'!$L$5</definedName>
+    <definedName name="moment" localSheetId="5">'Lätt ind kür'!$K$5</definedName>
+    <definedName name="moment" localSheetId="2">'Lätt lagkür 1'!$K$5</definedName>
+    <definedName name="moment" localSheetId="3">'Lätt lagkür 2'!$L$5</definedName>
+    <definedName name="result" localSheetId="1">'Lätt grund'!$K$38</definedName>
+    <definedName name="result" localSheetId="4">'Lätt ind grund'!$L$33</definedName>
+    <definedName name="result" localSheetId="5">'Lätt ind kür'!$K$35</definedName>
+    <definedName name="result" localSheetId="3">'Lätt lagkür 2'!$L$35</definedName>
+    <definedName name="result">'Lätt lagkür 1'!$K$38</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -427,7 +469,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -969,7 +1011,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1389,52 +1431,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1445,13 +1491,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1501,55 +1541,111 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1596,65 +1692,26 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1691,20 +1748,23 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1712,23 +1772,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1936,6 +1981,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1971,6 +2033,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2153,58 +2232,58 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="15.7109375" style="136" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="136"/>
+    <col min="1" max="18" width="15.73046875" style="136" customWidth="1"/>
+    <col min="19" max="16384" width="9.1328125" style="136"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="148" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="148" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A1" s="148" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="135" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="135" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="136" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="136" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="136" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="136" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="136" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="134" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="134" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A11" s="134" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="147" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="147" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A12" s="149"/>
       <c r="B12" s="149" t="s">
         <v>32</v>
@@ -2213,7 +2292,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="146" t="s">
         <v>100</v>
       </c>
@@ -2224,7 +2303,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="146" t="s">
         <v>102</v>
       </c>
@@ -2235,7 +2314,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="146" t="s">
         <v>103</v>
       </c>
@@ -2246,17 +2325,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A18" s="147" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="136" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="136" t="s">
         <v>118</v>
       </c>
@@ -2267,7 +2346,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="136" t="s">
         <v>117</v>
       </c>
@@ -2275,7 +2354,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="136" t="s">
         <v>57</v>
       </c>
@@ -2291,23 +2370,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A28" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="11" customWidth="1"/>
-    <col min="3" max="10" width="7.5703125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="11" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="11" customWidth="1"/>
+    <col min="1" max="2" width="8.73046875" style="11" customWidth="1"/>
+    <col min="3" max="10" width="7.59765625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="7.3984375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="7.73046875" style="11" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="27" t="s">
         <v>31</v>
       </c>
@@ -2319,7 +2398,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -2331,13 +2410,13 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="294"/>
+      <c r="D4" s="294"/>
       <c r="E4" s="42"/>
       <c r="G4" s="3"/>
       <c r="H4" s="7" t="s">
@@ -2347,14 +2426,14 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="188"/>
-      <c r="D5" s="188"/>
-      <c r="E5" s="188"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
       <c r="G5" s="3"/>
       <c r="H5" s="7" t="s">
         <v>13</v>
@@ -2363,7 +2442,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
@@ -2371,94 +2450,94 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="188"/>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188"/>
+      <c r="C7" s="229"/>
+      <c r="D7" s="229"/>
+      <c r="E7" s="229"/>
       <c r="G7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="190"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="191"/>
-    </row>
-    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="230"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="231"/>
+      <c r="K7" s="231"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="226"/>
       <c r="G8" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="180"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-    </row>
-    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="227"/>
+      <c r="I8" s="228"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="228"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="188"/>
-      <c r="D9" s="188"/>
-      <c r="E9" s="188"/>
+      <c r="C9" s="229"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
       <c r="G9" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="180"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-    </row>
-    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="227"/>
+      <c r="I9" s="228"/>
+      <c r="J9" s="228"/>
+      <c r="K9" s="228"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="188"/>
-      <c r="D10" s="188"/>
-      <c r="E10" s="188"/>
+      <c r="C10" s="229"/>
+      <c r="D10" s="229"/>
+      <c r="E10" s="229"/>
       <c r="G10" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="180"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-    </row>
-    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="227"/>
+      <c r="I10" s="228"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="228"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="180"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-    </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="227"/>
+      <c r="I11" s="228"/>
+      <c r="J11" s="228"/>
+      <c r="K11" s="228"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="G12" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="180"/>
-      <c r="I12" s="181"/>
-      <c r="J12" s="181"/>
-      <c r="K12" s="181"/>
-    </row>
-    <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="227"/>
+      <c r="I12" s="228"/>
+      <c r="J12" s="228"/>
+      <c r="K12" s="228"/>
+    </row>
+    <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="45">
         <v>1</v>
       </c>
@@ -2481,12 +2560,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="182" t="s">
+    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="232" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="183"/>
-      <c r="C15" s="184"/>
+      <c r="B15" s="233"/>
+      <c r="C15" s="234"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -2498,12 +2577,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="185" t="s">
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="218" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="186"/>
-      <c r="C16" s="187"/>
+      <c r="B16" s="219"/>
+      <c r="C16" s="220"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -2515,12 +2594,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="185" t="s">
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="186"/>
-      <c r="C17" s="187"/>
+      <c r="B17" s="219"/>
+      <c r="C17" s="220"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -2532,12 +2611,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="192" t="s">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="221" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="193"/>
-      <c r="C18" s="194"/>
+      <c r="B18" s="222"/>
+      <c r="C18" s="223"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -2549,12 +2628,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="185" t="s">
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="186"/>
-      <c r="C19" s="187"/>
+      <c r="B19" s="219"/>
+      <c r="C19" s="220"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -2566,12 +2645,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="185" t="s">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="218" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="186"/>
-      <c r="C20" s="187"/>
+      <c r="B20" s="219"/>
+      <c r="C20" s="220"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -2583,10 +2662,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J21" s="29"/>
     </row>
-    <row r="22" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>0</v>
       </c>
@@ -2603,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="E23" s="16"/>
       <c r="G23" s="17" t="s">
@@ -2618,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2627,12 +2706,12 @@
       <c r="F24" s="15"/>
       <c r="J24" s="19"/>
     </row>
-    <row r="25" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J25" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G26" s="21" t="s">
         <v>27</v>
       </c>
@@ -2643,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E27" s="31"/>
       <c r="G27" s="30"/>
       <c r="H27" s="30"/>
@@ -2651,7 +2730,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="25"/>
     </row>
-    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A28" s="47" t="s">
         <v>3</v>
       </c>
@@ -2660,91 +2739,91 @@
       <c r="D28" s="48"/>
       <c r="E28" s="48"/>
       <c r="F28" s="48"/>
-      <c r="G28" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="196"/>
+      <c r="G28" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="225"/>
       <c r="I28" s="197" t="s">
         <v>7</v>
       </c>
       <c r="J28" s="198"/>
       <c r="K28" s="199"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="200" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="203" t="s">
+      <c r="B29" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="203" t="s">
+      <c r="C29" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="203"/>
-      <c r="E29" s="205" t="s">
+      <c r="D29" s="201"/>
+      <c r="E29" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="206"/>
-      <c r="G29" s="207"/>
-      <c r="H29" s="208"/>
-      <c r="I29" s="209">
+      <c r="F29" s="204"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="206"/>
+      <c r="I29" s="207">
         <v>0.2</v>
       </c>
-      <c r="J29" s="212"/>
-      <c r="K29" s="214">
+      <c r="J29" s="210"/>
+      <c r="K29" s="212">
         <f>J29*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="201"/>
-      <c r="B30" s="203"/>
-      <c r="C30" s="203" t="s">
+    <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="200"/>
+      <c r="B30" s="201"/>
+      <c r="C30" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="203"/>
-      <c r="E30" s="216" t="s">
+      <c r="D30" s="201"/>
+      <c r="E30" s="214" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="217"/>
-      <c r="G30" s="218"/>
-      <c r="H30" s="219"/>
-      <c r="I30" s="210"/>
-      <c r="J30" s="212"/>
-      <c r="K30" s="214"/>
-    </row>
-    <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="202"/>
-      <c r="B31" s="204"/>
-      <c r="C31" s="204" t="s">
+      <c r="F30" s="215"/>
+      <c r="G30" s="190"/>
+      <c r="H30" s="191"/>
+      <c r="I30" s="208"/>
+      <c r="J30" s="210"/>
+      <c r="K30" s="212"/>
+    </row>
+    <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="184"/>
+      <c r="B31" s="202"/>
+      <c r="C31" s="202" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="204"/>
-      <c r="E31" s="216" t="s">
+      <c r="D31" s="202"/>
+      <c r="E31" s="214" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="217"/>
-      <c r="G31" s="220"/>
-      <c r="H31" s="221"/>
-      <c r="I31" s="211"/>
-      <c r="J31" s="213"/>
-      <c r="K31" s="215"/>
-    </row>
-    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="200" t="s">
+      <c r="F31" s="215"/>
+      <c r="G31" s="216"/>
+      <c r="H31" s="217"/>
+      <c r="I31" s="209"/>
+      <c r="J31" s="211"/>
+      <c r="K31" s="213"/>
+    </row>
+    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="225" t="s">
+      <c r="B32" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="226"/>
-      <c r="D32" s="227"/>
-      <c r="E32" s="228" t="s">
+      <c r="C32" s="186"/>
+      <c r="D32" s="187"/>
+      <c r="E32" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="229"/>
-      <c r="G32" s="218"/>
-      <c r="H32" s="219"/>
+      <c r="F32" s="189"/>
+      <c r="G32" s="190"/>
+      <c r="H32" s="191"/>
       <c r="I32" s="49">
         <v>0.4</v>
       </c>
@@ -2754,19 +2833,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="202"/>
-      <c r="B33" s="230" t="s">
+    <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="184"/>
+      <c r="B33" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="231"/>
-      <c r="D33" s="232"/>
-      <c r="E33" s="233" t="s">
+      <c r="C33" s="193"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="234"/>
-      <c r="G33" s="218"/>
-      <c r="H33" s="219"/>
+      <c r="F33" s="196"/>
+      <c r="G33" s="190"/>
+      <c r="H33" s="191"/>
       <c r="I33" s="49">
         <v>0.4</v>
       </c>
@@ -2776,27 +2855,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="222" t="s">
+      <c r="B34" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="223"/>
-      <c r="D34" s="223"/>
-      <c r="E34" s="223"/>
-      <c r="F34" s="223"/>
-      <c r="G34" s="223"/>
-      <c r="H34" s="223"/>
-      <c r="I34" s="224"/>
+      <c r="C34" s="181"/>
+      <c r="D34" s="181"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="181"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="181"/>
+      <c r="I34" s="182"/>
       <c r="J34" s="60"/>
       <c r="K34" s="154">
         <f>J34</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="52"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
@@ -2814,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="52"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
@@ -2832,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="52"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
@@ -2850,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E38" s="31"/>
       <c r="G38" s="30"/>
       <c r="H38" s="37"/>
@@ -2865,8 +2944,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>28</v>
       </c>
@@ -2882,7 +2961,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E41" s="31"/>
       <c r="G41" s="30"/>
       <c r="H41" s="30"/>
@@ -2890,18 +2969,29 @@
       <c r="J41" s="17"/>
       <c r="K41" s="25"/>
     </row>
-    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
+  <mergeCells count="42">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="B29:B31"/>
@@ -2917,24 +3007,14 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
   </mergeCells>
   <conditionalFormatting sqref="K29:K37">
     <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
@@ -2960,24 +3040,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:G25"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="11" customWidth="1"/>
-    <col min="2" max="7" width="7.42578125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" style="11" customWidth="1"/>
+    <col min="2" max="7" width="7.3984375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="6.3984375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="7.265625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="5.1328125" style="11" customWidth="1"/>
     <col min="11" max="11" width="10" style="11" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="11" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="11"/>
+    <col min="12" max="12" width="7.265625" style="11" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="27" t="s">
         <v>98</v>
       </c>
@@ -2989,7 +3069,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
@@ -3001,13 +3081,13 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="122"/>
       <c r="G4" s="3"/>
       <c r="H4" s="7" t="s">
@@ -3017,14 +3097,14 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="188"/>
-      <c r="D5" s="188"/>
-      <c r="E5" s="188"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
       <c r="G5" s="3"/>
       <c r="H5" s="7" t="s">
         <v>13</v>
@@ -3033,7 +3113,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
@@ -3041,94 +3121,94 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="188"/>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188"/>
+      <c r="C7" s="229"/>
+      <c r="D7" s="229"/>
+      <c r="E7" s="229"/>
       <c r="G7" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="190"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="191"/>
-    </row>
-    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="230"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="231"/>
+      <c r="K7" s="231"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="226"/>
       <c r="G8" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="180"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-    </row>
-    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="227"/>
+      <c r="I8" s="228"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="228"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="188"/>
-      <c r="D9" s="188"/>
-      <c r="E9" s="188"/>
+      <c r="C9" s="229"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
       <c r="G9" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="180"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-    </row>
-    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="227"/>
+      <c r="I9" s="228"/>
+      <c r="J9" s="228"/>
+      <c r="K9" s="228"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="188"/>
-      <c r="D10" s="188"/>
-      <c r="E10" s="188"/>
+      <c r="C10" s="229"/>
+      <c r="D10" s="229"/>
+      <c r="E10" s="229"/>
       <c r="G10" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="180"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-    </row>
-    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="227"/>
+      <c r="I10" s="228"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="228"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="180"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-    </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="227"/>
+      <c r="I11" s="228"/>
+      <c r="J11" s="228"/>
+      <c r="K11" s="228"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="G12" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="180"/>
-      <c r="I12" s="181"/>
-      <c r="J12" s="181"/>
-      <c r="K12" s="181"/>
-    </row>
-    <row r="13" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="227"/>
+      <c r="I12" s="228"/>
+      <c r="J12" s="228"/>
+      <c r="K12" s="228"/>
+    </row>
+    <row r="13" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
         <v>3</v>
       </c>
@@ -3137,91 +3217,91 @@
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="48"/>
-      <c r="G14" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="196"/>
+      <c r="G14" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="225"/>
       <c r="I14" s="197" t="s">
         <v>7</v>
       </c>
       <c r="J14" s="198"/>
       <c r="K14" s="199"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="250" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="235" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="263" t="s">
+      <c r="B15" s="238" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="263" t="s">
+      <c r="C15" s="238" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="263"/>
-      <c r="E15" s="255" t="s">
+      <c r="D15" s="238"/>
+      <c r="E15" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="265"/>
-      <c r="G15" s="207"/>
-      <c r="H15" s="208"/>
-      <c r="I15" s="209">
+      <c r="F15" s="241"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="206"/>
+      <c r="I15" s="207">
         <v>0.2</v>
       </c>
-      <c r="J15" s="212"/>
-      <c r="K15" s="214">
+      <c r="J15" s="210"/>
+      <c r="K15" s="212">
         <f>J15*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="262"/>
-      <c r="B16" s="263"/>
-      <c r="C16" s="263" t="s">
+    <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="236"/>
+      <c r="B16" s="238"/>
+      <c r="C16" s="238" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="263"/>
-      <c r="E16" s="266" t="s">
+      <c r="D16" s="238"/>
+      <c r="E16" s="242" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="267"/>
-      <c r="G16" s="218"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="210"/>
-      <c r="J16" s="212"/>
-      <c r="K16" s="214"/>
-    </row>
-    <row r="17" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="251"/>
-      <c r="B17" s="264"/>
-      <c r="C17" s="264" t="s">
+      <c r="F16" s="243"/>
+      <c r="G16" s="190"/>
+      <c r="H16" s="191"/>
+      <c r="I16" s="208"/>
+      <c r="J16" s="210"/>
+      <c r="K16" s="212"/>
+    </row>
+    <row r="17" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="237"/>
+      <c r="B17" s="239"/>
+      <c r="C17" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="264"/>
-      <c r="E17" s="266" t="s">
+      <c r="D17" s="239"/>
+      <c r="E17" s="242" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="267"/>
-      <c r="G17" s="220"/>
-      <c r="H17" s="221"/>
-      <c r="I17" s="211"/>
-      <c r="J17" s="213"/>
-      <c r="K17" s="215"/>
-    </row>
-    <row r="18" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="250" t="s">
+      <c r="F17" s="243"/>
+      <c r="G17" s="216"/>
+      <c r="H17" s="217"/>
+      <c r="I17" s="209"/>
+      <c r="J17" s="211"/>
+      <c r="K17" s="213"/>
+    </row>
+    <row r="18" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="252" t="s">
+      <c r="B18" s="244" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="253"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="255" t="s">
+      <c r="C18" s="245"/>
+      <c r="D18" s="246"/>
+      <c r="E18" s="240" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="256"/>
-      <c r="G18" s="218"/>
-      <c r="H18" s="219"/>
+      <c r="F18" s="247"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="191"/>
       <c r="I18" s="120">
         <v>0.4</v>
       </c>
@@ -3232,19 +3312,19 @@
       </c>
       <c r="L18" s="26"/>
     </row>
-    <row r="19" spans="1:12" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="251"/>
-      <c r="B19" s="257" t="s">
+    <row r="19" spans="1:12" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="237"/>
+      <c r="B19" s="248" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="258"/>
-      <c r="D19" s="259"/>
-      <c r="E19" s="260" t="s">
+      <c r="C19" s="249"/>
+      <c r="D19" s="250"/>
+      <c r="E19" s="251" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="261"/>
-      <c r="G19" s="218"/>
-      <c r="H19" s="219"/>
+      <c r="F19" s="252"/>
+      <c r="G19" s="190"/>
+      <c r="H19" s="191"/>
       <c r="I19" s="120">
         <v>0.4</v>
       </c>
@@ -3254,24 +3334,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="13.15" x14ac:dyDescent="0.3">
       <c r="A20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="223"/>
-      <c r="D20" s="223"/>
-      <c r="E20" s="223"/>
-      <c r="F20" s="223"/>
-      <c r="G20" s="223"/>
-      <c r="H20" s="223"/>
-      <c r="I20" s="224"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="182"/>
       <c r="J20" s="121"/>
       <c r="K20" s="155"/>
     </row>
-    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="52"/>
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
@@ -3289,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="54" t="s">
         <v>57</v>
       </c>
@@ -3306,7 +3386,7 @@
       <c r="J22" s="33"/>
       <c r="K22" s="36"/>
     </row>
-    <row r="23" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="52"/>
       <c r="B23" s="46">
         <v>1</v>
@@ -3330,7 +3410,7 @@
       <c r="J23" s="33"/>
       <c r="K23" s="36"/>
     </row>
-    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="55" t="s">
         <v>90</v>
       </c>
@@ -3345,7 +3425,7 @@
       <c r="J24" s="33"/>
       <c r="K24" s="36"/>
     </row>
-    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="55" t="s">
         <v>89</v>
       </c>
@@ -3362,7 +3442,7 @@
       <c r="J25" s="33"/>
       <c r="K25" s="36"/>
     </row>
-    <row r="26" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="52"/>
       <c r="B26" s="161">
         <f t="shared" ref="B26:G26" si="0">SUM(B24:B25)</f>
@@ -3396,7 +3476,7 @@
       <c r="J26" s="33"/>
       <c r="K26" s="36"/>
     </row>
-    <row r="27" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="52"/>
       <c r="B27" s="52"/>
       <c r="C27" s="52"/>
@@ -3418,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
       <c r="D28" s="52"/>
@@ -3430,89 +3510,89 @@
       <c r="J28" s="33"/>
       <c r="K28" s="33"/>
     </row>
-    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="240" t="s">
+    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="241"/>
-      <c r="C29" s="241"/>
-      <c r="D29" s="241"/>
-      <c r="E29" s="241"/>
-      <c r="F29" s="241"/>
-      <c r="G29" s="241"/>
-      <c r="H29" s="241"/>
-      <c r="I29" s="241"/>
-      <c r="J29" s="241"/>
-      <c r="K29" s="242"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="243"/>
-      <c r="B30" s="244"/>
-      <c r="C30" s="244"/>
-      <c r="D30" s="244"/>
-      <c r="E30" s="244"/>
-      <c r="F30" s="244"/>
-      <c r="G30" s="244"/>
-      <c r="H30" s="244"/>
-      <c r="I30" s="244"/>
-      <c r="J30" s="244"/>
-      <c r="K30" s="245"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="243"/>
-      <c r="B31" s="244"/>
-      <c r="C31" s="244"/>
-      <c r="D31" s="244"/>
-      <c r="E31" s="244"/>
-      <c r="F31" s="244"/>
-      <c r="G31" s="244"/>
-      <c r="H31" s="244"/>
-      <c r="I31" s="244"/>
-      <c r="J31" s="244"/>
-      <c r="K31" s="245"/>
-    </row>
-    <row r="32" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="243"/>
-      <c r="B32" s="244"/>
-      <c r="C32" s="244"/>
-      <c r="D32" s="244"/>
-      <c r="E32" s="244"/>
-      <c r="F32" s="244"/>
-      <c r="G32" s="244"/>
-      <c r="H32" s="244"/>
-      <c r="I32" s="244"/>
-      <c r="J32" s="244"/>
-      <c r="K32" s="245"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="246"/>
-      <c r="B33" s="247"/>
-      <c r="C33" s="247"/>
-      <c r="D33" s="247"/>
-      <c r="E33" s="247"/>
-      <c r="F33" s="247"/>
-      <c r="G33" s="247"/>
-      <c r="H33" s="247"/>
-      <c r="I33" s="247"/>
-      <c r="J33" s="247"/>
-      <c r="K33" s="248"/>
-    </row>
-    <row r="34" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="238" t="s">
+      <c r="B29" s="259"/>
+      <c r="C29" s="259"/>
+      <c r="D29" s="259"/>
+      <c r="E29" s="259"/>
+      <c r="F29" s="259"/>
+      <c r="G29" s="259"/>
+      <c r="H29" s="259"/>
+      <c r="I29" s="259"/>
+      <c r="J29" s="259"/>
+      <c r="K29" s="260"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="261"/>
+      <c r="B30" s="262"/>
+      <c r="C30" s="262"/>
+      <c r="D30" s="262"/>
+      <c r="E30" s="262"/>
+      <c r="F30" s="262"/>
+      <c r="G30" s="262"/>
+      <c r="H30" s="262"/>
+      <c r="I30" s="262"/>
+      <c r="J30" s="262"/>
+      <c r="K30" s="263"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="261"/>
+      <c r="B31" s="262"/>
+      <c r="C31" s="262"/>
+      <c r="D31" s="262"/>
+      <c r="E31" s="262"/>
+      <c r="F31" s="262"/>
+      <c r="G31" s="262"/>
+      <c r="H31" s="262"/>
+      <c r="I31" s="262"/>
+      <c r="J31" s="262"/>
+      <c r="K31" s="263"/>
+    </row>
+    <row r="32" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="261"/>
+      <c r="B32" s="262"/>
+      <c r="C32" s="262"/>
+      <c r="D32" s="262"/>
+      <c r="E32" s="262"/>
+      <c r="F32" s="262"/>
+      <c r="G32" s="262"/>
+      <c r="H32" s="262"/>
+      <c r="I32" s="262"/>
+      <c r="J32" s="262"/>
+      <c r="K32" s="263"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="264"/>
+      <c r="B33" s="265"/>
+      <c r="C33" s="265"/>
+      <c r="D33" s="265"/>
+      <c r="E33" s="265"/>
+      <c r="F33" s="265"/>
+      <c r="G33" s="265"/>
+      <c r="H33" s="265"/>
+      <c r="I33" s="265"/>
+      <c r="J33" s="265"/>
+      <c r="K33" s="266"/>
+    </row>
+    <row r="34" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="256" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="238"/>
-      <c r="C35" s="238"/>
-      <c r="D35" s="238"/>
-      <c r="E35" s="238"/>
-      <c r="F35" s="238"/>
-      <c r="G35" s="238"/>
-      <c r="H35" s="249">
+      <c r="B35" s="256"/>
+      <c r="C35" s="256"/>
+      <c r="D35" s="256"/>
+      <c r="E35" s="256"/>
+      <c r="F35" s="256"/>
+      <c r="G35" s="256"/>
+      <c r="H35" s="267">
         <f>K27</f>
         <v>0</v>
       </c>
-      <c r="I35" s="249"/>
+      <c r="I35" s="267"/>
       <c r="J35" s="34" t="s">
         <v>47</v>
       </c>
@@ -3521,21 +3601,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="238" t="s">
+    <row r="36" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="256" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="238"/>
-      <c r="C36" s="238"/>
-      <c r="D36" s="238"/>
-      <c r="E36" s="238"/>
-      <c r="F36" s="238"/>
-      <c r="G36" s="238"/>
-      <c r="H36" s="239">
+      <c r="B36" s="256"/>
+      <c r="C36" s="256"/>
+      <c r="D36" s="256"/>
+      <c r="E36" s="256"/>
+      <c r="F36" s="256"/>
+      <c r="G36" s="256"/>
+      <c r="H36" s="257">
         <f>K21</f>
         <v>0</v>
       </c>
-      <c r="I36" s="239"/>
+      <c r="I36" s="257"/>
       <c r="J36" s="57" t="s">
         <v>63</v>
       </c>
@@ -3544,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="52"/>
       <c r="E37" s="28"/>
       <c r="H37" s="1"/>
@@ -3557,25 +3637,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="52"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
       <c r="D38" s="52"/>
-      <c r="E38" s="235" t="s">
+      <c r="E38" s="253" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="236"/>
-      <c r="G38" s="236"/>
-      <c r="H38" s="236"/>
-      <c r="I38" s="236"/>
-      <c r="J38" s="237"/>
+      <c r="F38" s="254"/>
+      <c r="G38" s="254"/>
+      <c r="H38" s="254"/>
+      <c r="I38" s="254"/>
+      <c r="J38" s="255"/>
       <c r="K38" s="58">
         <f>K37/4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="52"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
@@ -3588,7 +3668,7 @@
       <c r="J39" s="157"/>
       <c r="K39" s="145"/>
     </row>
-    <row r="40" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A40" s="52"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
@@ -3601,7 +3681,7 @@
       <c r="J40" s="28"/>
       <c r="K40" s="59"/>
     </row>
-    <row r="41" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A41" s="52"/>
       <c r="B41" s="52"/>
       <c r="C41" s="52"/>
@@ -3614,7 +3694,7 @@
       <c r="J41" s="28"/>
       <c r="K41" s="59"/>
     </row>
-    <row r="42" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A42" s="52"/>
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
@@ -3627,7 +3707,7 @@
       <c r="J42" s="28"/>
       <c r="K42" s="59"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
@@ -3643,7 +3723,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E45" s="31"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
@@ -3652,18 +3732,22 @@
       <c r="K45" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
+  <mergeCells count="42">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="A29:K33"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="A15:A17"/>
@@ -3680,20 +3764,17 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="A29:K33"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
   </mergeCells>
   <conditionalFormatting sqref="H36:I36 K15:K42">
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
@@ -3722,27 +3803,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:J32"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="11" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="11"/>
-    <col min="4" max="4" width="2.7109375" style="11" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="11" customWidth="1"/>
-    <col min="10" max="11" width="7.28515625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="11" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="11" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="8.265625" style="11" customWidth="1"/>
+    <col min="2" max="3" width="9.1328125" style="11"/>
+    <col min="4" max="4" width="2.73046875" style="11" customWidth="1"/>
+    <col min="5" max="6" width="7.265625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="6.86328125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="6.59765625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="6.1328125" style="11" customWidth="1"/>
+    <col min="10" max="11" width="7.265625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="8.73046875" style="11" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="11" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="27" t="s">
         <v>97</v>
       </c>
@@ -3754,7 +3835,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
@@ -3766,14 +3847,14 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
       <c r="F4" s="42"/>
       <c r="H4" s="3"/>
       <c r="I4" s="7" t="s">
@@ -3783,15 +3864,15 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="188"/>
-      <c r="D5" s="188"/>
-      <c r="E5" s="188"/>
-      <c r="F5" s="188"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
       <c r="H5" s="3"/>
       <c r="I5" s="7" t="s">
         <v>13</v>
@@ -3800,7 +3881,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
@@ -3808,98 +3889,98 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="188"/>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188"/>
-      <c r="F7" s="188"/>
+      <c r="C7" s="229"/>
+      <c r="D7" s="229"/>
+      <c r="E7" s="229"/>
+      <c r="F7" s="229"/>
       <c r="H7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="190"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="191"/>
-      <c r="L7" s="191"/>
-    </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="230"/>
+      <c r="J7" s="231"/>
+      <c r="K7" s="231"/>
+      <c r="L7" s="231"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
-      <c r="F8" s="189"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="226"/>
+      <c r="F8" s="226"/>
       <c r="H8" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="180"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="181"/>
-    </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="227"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="228"/>
+      <c r="L8" s="228"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="188"/>
-      <c r="D9" s="188"/>
-      <c r="E9" s="188"/>
-      <c r="F9" s="188"/>
+      <c r="C9" s="229"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
+      <c r="F9" s="229"/>
       <c r="H9" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="180"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="181"/>
-    </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="227"/>
+      <c r="J9" s="228"/>
+      <c r="K9" s="228"/>
+      <c r="L9" s="228"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="188"/>
-      <c r="D10" s="188"/>
-      <c r="E10" s="188"/>
-      <c r="F10" s="188"/>
+      <c r="C10" s="229"/>
+      <c r="D10" s="229"/>
+      <c r="E10" s="229"/>
+      <c r="F10" s="229"/>
       <c r="H10" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="180"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="181"/>
-    </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="227"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="228"/>
+      <c r="L10" s="228"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="180"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="181"/>
-    </row>
-    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="227"/>
+      <c r="J11" s="228"/>
+      <c r="K11" s="228"/>
+      <c r="L11" s="228"/>
+    </row>
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="H12" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="180"/>
-      <c r="J12" s="181"/>
-      <c r="K12" s="181"/>
-      <c r="L12" s="181"/>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="227"/>
+      <c r="J12" s="228"/>
+      <c r="K12" s="228"/>
+      <c r="L12" s="228"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">
         <v>3</v>
       </c>
@@ -3909,95 +3990,95 @@
       <c r="E14" s="48"/>
       <c r="F14" s="48"/>
       <c r="G14" s="48"/>
-      <c r="H14" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="196"/>
+      <c r="H14" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="225"/>
       <c r="J14" s="197" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="198"/>
       <c r="L14" s="199"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="250" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="235" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="263" t="s">
+      <c r="B15" s="238" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="263" t="s">
+      <c r="C15" s="238" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="263"/>
-      <c r="E15" s="263"/>
-      <c r="F15" s="255" t="s">
+      <c r="D15" s="238"/>
+      <c r="E15" s="238"/>
+      <c r="F15" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="265"/>
-      <c r="H15" s="207"/>
-      <c r="I15" s="208"/>
-      <c r="J15" s="209">
+      <c r="G15" s="241"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="206"/>
+      <c r="J15" s="207">
         <v>0.2</v>
       </c>
-      <c r="K15" s="212"/>
-      <c r="L15" s="214">
+      <c r="K15" s="210"/>
+      <c r="L15" s="212">
         <f>K15*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="262"/>
-      <c r="B16" s="263"/>
-      <c r="C16" s="263" t="s">
+    <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="236"/>
+      <c r="B16" s="238"/>
+      <c r="C16" s="238" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="263"/>
-      <c r="E16" s="263"/>
-      <c r="F16" s="266" t="s">
+      <c r="D16" s="238"/>
+      <c r="E16" s="238"/>
+      <c r="F16" s="242" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="267"/>
-      <c r="H16" s="218"/>
-      <c r="I16" s="219"/>
-      <c r="J16" s="210"/>
-      <c r="K16" s="212"/>
-      <c r="L16" s="214"/>
-    </row>
-    <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="251"/>
-      <c r="B17" s="264"/>
-      <c r="C17" s="264" t="s">
+      <c r="G16" s="243"/>
+      <c r="H16" s="190"/>
+      <c r="I16" s="191"/>
+      <c r="J16" s="208"/>
+      <c r="K16" s="210"/>
+      <c r="L16" s="212"/>
+    </row>
+    <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="237"/>
+      <c r="B17" s="239"/>
+      <c r="C17" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="264"/>
-      <c r="E17" s="264"/>
-      <c r="F17" s="266" t="s">
+      <c r="D17" s="239"/>
+      <c r="E17" s="239"/>
+      <c r="F17" s="242" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="267"/>
-      <c r="H17" s="220"/>
-      <c r="I17" s="221"/>
-      <c r="J17" s="211"/>
-      <c r="K17" s="213"/>
-      <c r="L17" s="215"/>
-    </row>
-    <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="250" t="s">
+      <c r="G17" s="243"/>
+      <c r="H17" s="216"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="209"/>
+      <c r="K17" s="211"/>
+      <c r="L17" s="213"/>
+    </row>
+    <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="252" t="s">
+      <c r="B18" s="244" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="253"/>
-      <c r="D18" s="253"/>
-      <c r="E18" s="254"/>
-      <c r="F18" s="255" t="s">
+      <c r="C18" s="245"/>
+      <c r="D18" s="245"/>
+      <c r="E18" s="246"/>
+      <c r="F18" s="240" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="256"/>
-      <c r="H18" s="218"/>
-      <c r="I18" s="219"/>
+      <c r="G18" s="247"/>
+      <c r="H18" s="190"/>
+      <c r="I18" s="191"/>
       <c r="J18" s="49">
         <v>0.4</v>
       </c>
@@ -4008,20 +4089,20 @@
       </c>
       <c r="M18" s="26"/>
     </row>
-    <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="251"/>
-      <c r="B19" s="257" t="s">
+    <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="237"/>
+      <c r="B19" s="248" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="258"/>
-      <c r="D19" s="258"/>
-      <c r="E19" s="259"/>
-      <c r="F19" s="260" t="s">
+      <c r="C19" s="249"/>
+      <c r="D19" s="249"/>
+      <c r="E19" s="250"/>
+      <c r="F19" s="251" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="261"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="219"/>
+      <c r="G19" s="252"/>
+      <c r="H19" s="190"/>
+      <c r="I19" s="191"/>
       <c r="J19" s="49">
         <v>0.4</v>
       </c>
@@ -4031,25 +4112,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="13.15" x14ac:dyDescent="0.3">
       <c r="A20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="180" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="223"/>
-      <c r="D20" s="223"/>
-      <c r="E20" s="223"/>
-      <c r="F20" s="223"/>
-      <c r="G20" s="223"/>
-      <c r="H20" s="223"/>
-      <c r="I20" s="223"/>
-      <c r="J20" s="224"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="182"/>
       <c r="K20" s="50"/>
       <c r="L20" s="155"/>
     </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="52"/>
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
@@ -4066,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="54" t="s">
         <v>57</v>
       </c>
@@ -4082,89 +4163,89 @@
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="240" t="s">
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="241"/>
-      <c r="C23" s="241"/>
-      <c r="D23" s="241"/>
-      <c r="E23" s="241"/>
-      <c r="F23" s="241"/>
-      <c r="G23" s="241"/>
-      <c r="H23" s="241"/>
-      <c r="I23" s="241"/>
-      <c r="J23" s="241"/>
-      <c r="K23" s="241"/>
-      <c r="L23" s="242"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="243"/>
-      <c r="B24" s="244"/>
-      <c r="C24" s="244"/>
-      <c r="D24" s="244"/>
-      <c r="E24" s="244"/>
-      <c r="F24" s="244"/>
-      <c r="G24" s="244"/>
-      <c r="H24" s="244"/>
-      <c r="I24" s="244"/>
-      <c r="J24" s="244"/>
-      <c r="K24" s="244"/>
-      <c r="L24" s="245"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="243"/>
-      <c r="B25" s="244"/>
-      <c r="C25" s="244"/>
-      <c r="D25" s="244"/>
-      <c r="E25" s="244"/>
-      <c r="F25" s="244"/>
-      <c r="G25" s="244"/>
-      <c r="H25" s="244"/>
-      <c r="I25" s="244"/>
-      <c r="J25" s="244"/>
-      <c r="K25" s="244"/>
-      <c r="L25" s="245"/>
-    </row>
-    <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="243"/>
-      <c r="B26" s="244"/>
-      <c r="C26" s="244"/>
-      <c r="D26" s="244"/>
-      <c r="E26" s="244"/>
-      <c r="F26" s="244"/>
-      <c r="G26" s="244"/>
-      <c r="H26" s="244"/>
-      <c r="I26" s="244"/>
-      <c r="J26" s="244"/>
-      <c r="K26" s="244"/>
-      <c r="L26" s="245"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="246"/>
-      <c r="B27" s="247"/>
-      <c r="C27" s="247"/>
-      <c r="D27" s="247"/>
-      <c r="E27" s="247"/>
-      <c r="F27" s="247"/>
-      <c r="G27" s="247"/>
-      <c r="H27" s="247"/>
-      <c r="I27" s="247"/>
-      <c r="J27" s="247"/>
-      <c r="K27" s="247"/>
-      <c r="L27" s="248"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="238" t="s">
+      <c r="B23" s="259"/>
+      <c r="C23" s="259"/>
+      <c r="D23" s="259"/>
+      <c r="E23" s="259"/>
+      <c r="F23" s="259"/>
+      <c r="G23" s="259"/>
+      <c r="H23" s="259"/>
+      <c r="I23" s="259"/>
+      <c r="J23" s="259"/>
+      <c r="K23" s="259"/>
+      <c r="L23" s="260"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="261"/>
+      <c r="B24" s="262"/>
+      <c r="C24" s="262"/>
+      <c r="D24" s="262"/>
+      <c r="E24" s="262"/>
+      <c r="F24" s="262"/>
+      <c r="G24" s="262"/>
+      <c r="H24" s="262"/>
+      <c r="I24" s="262"/>
+      <c r="J24" s="262"/>
+      <c r="K24" s="262"/>
+      <c r="L24" s="263"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="261"/>
+      <c r="B25" s="262"/>
+      <c r="C25" s="262"/>
+      <c r="D25" s="262"/>
+      <c r="E25" s="262"/>
+      <c r="F25" s="262"/>
+      <c r="G25" s="262"/>
+      <c r="H25" s="262"/>
+      <c r="I25" s="262"/>
+      <c r="J25" s="262"/>
+      <c r="K25" s="262"/>
+      <c r="L25" s="263"/>
+    </row>
+    <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="261"/>
+      <c r="B26" s="262"/>
+      <c r="C26" s="262"/>
+      <c r="D26" s="262"/>
+      <c r="E26" s="262"/>
+      <c r="F26" s="262"/>
+      <c r="G26" s="262"/>
+      <c r="H26" s="262"/>
+      <c r="I26" s="262"/>
+      <c r="J26" s="262"/>
+      <c r="K26" s="262"/>
+      <c r="L26" s="263"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="264"/>
+      <c r="B27" s="265"/>
+      <c r="C27" s="265"/>
+      <c r="D27" s="265"/>
+      <c r="E27" s="265"/>
+      <c r="F27" s="265"/>
+      <c r="G27" s="265"/>
+      <c r="H27" s="265"/>
+      <c r="I27" s="265"/>
+      <c r="J27" s="265"/>
+      <c r="K27" s="265"/>
+      <c r="L27" s="266"/>
+    </row>
+    <row r="29" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="256" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="238"/>
-      <c r="C29" s="238"/>
-      <c r="D29" s="238"/>
-      <c r="E29" s="238"/>
-      <c r="F29" s="238"/>
-      <c r="G29" s="238"/>
-      <c r="H29" s="238"/>
+      <c r="B29" s="256"/>
+      <c r="C29" s="256"/>
+      <c r="D29" s="256"/>
+      <c r="E29" s="256"/>
+      <c r="F29" s="256"/>
+      <c r="G29" s="256"/>
+      <c r="H29" s="256"/>
       <c r="I29" s="268"/>
       <c r="J29" s="268"/>
       <c r="K29" s="65" t="s">
@@ -4175,17 +4256,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="238" t="s">
+    <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="256" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="238"/>
-      <c r="C30" s="238"/>
-      <c r="D30" s="238"/>
-      <c r="E30" s="238"/>
-      <c r="F30" s="238"/>
-      <c r="G30" s="238"/>
-      <c r="H30" s="238"/>
+      <c r="B30" s="256"/>
+      <c r="C30" s="256"/>
+      <c r="D30" s="256"/>
+      <c r="E30" s="256"/>
+      <c r="F30" s="256"/>
+      <c r="G30" s="256"/>
+      <c r="H30" s="256"/>
       <c r="I30" s="268"/>
       <c r="J30" s="268"/>
       <c r="K30" s="45" t="s">
@@ -4196,17 +4277,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="238" t="s">
+    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="256" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="238"/>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="238"/>
-      <c r="G31" s="238"/>
-      <c r="H31" s="238"/>
+      <c r="B31" s="256"/>
+      <c r="C31" s="256"/>
+      <c r="D31" s="256"/>
+      <c r="E31" s="256"/>
+      <c r="F31" s="256"/>
+      <c r="G31" s="256"/>
+      <c r="H31" s="256"/>
       <c r="I31" s="268"/>
       <c r="J31" s="268"/>
       <c r="K31" s="150" t="s">
@@ -4217,17 +4298,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="238" t="s">
+    <row r="32" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="256" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="238"/>
-      <c r="C32" s="238"/>
-      <c r="D32" s="238"/>
-      <c r="E32" s="238"/>
-      <c r="F32" s="238"/>
-      <c r="G32" s="238"/>
-      <c r="H32" s="238"/>
+      <c r="B32" s="256"/>
+      <c r="C32" s="256"/>
+      <c r="D32" s="256"/>
+      <c r="E32" s="256"/>
+      <c r="F32" s="256"/>
+      <c r="G32" s="256"/>
+      <c r="H32" s="256"/>
       <c r="I32" s="268"/>
       <c r="J32" s="268"/>
       <c r="K32" s="45" t="s">
@@ -4238,22 +4319,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="238" t="s">
+    <row r="33" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="256" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="238"/>
-      <c r="C33" s="238"/>
-      <c r="D33" s="238"/>
-      <c r="E33" s="238"/>
-      <c r="F33" s="238"/>
-      <c r="G33" s="238"/>
-      <c r="H33" s="238"/>
-      <c r="I33" s="239">
+      <c r="B33" s="256"/>
+      <c r="C33" s="256"/>
+      <c r="D33" s="256"/>
+      <c r="E33" s="256"/>
+      <c r="F33" s="256"/>
+      <c r="G33" s="256"/>
+      <c r="H33" s="256"/>
+      <c r="I33" s="257">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="J33" s="239"/>
+      <c r="J33" s="257"/>
       <c r="K33" s="150" t="s">
         <v>110</v>
       </c>
@@ -4262,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="52"/>
       <c r="F34" s="28"/>
       <c r="I34" s="1"/>
@@ -4275,26 +4356,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="52"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
       <c r="D35" s="52"/>
       <c r="E35" s="52"/>
-      <c r="F35" s="235" t="s">
+      <c r="F35" s="253" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="236"/>
-      <c r="H35" s="236"/>
-      <c r="I35" s="236"/>
-      <c r="J35" s="236"/>
-      <c r="K35" s="237"/>
+      <c r="G35" s="254"/>
+      <c r="H35" s="254"/>
+      <c r="I35" s="254"/>
+      <c r="J35" s="254"/>
+      <c r="K35" s="255"/>
       <c r="L35" s="58">
         <f>L34/10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A36" s="52"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
@@ -4308,7 +4389,7 @@
       <c r="K36" s="28"/>
       <c r="L36" s="59"/>
     </row>
-    <row r="37" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A37" s="52"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
@@ -4322,7 +4403,7 @@
       <c r="K37" s="28"/>
       <c r="L37" s="59"/>
     </row>
-    <row r="38" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A38" s="52"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
@@ -4336,7 +4417,7 @@
       <c r="K38" s="28"/>
       <c r="L38" s="59"/>
     </row>
-    <row r="39" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A39" s="52"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
@@ -4350,7 +4431,7 @@
       <c r="K39" s="28"/>
       <c r="L39" s="59"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F40" s="31"/>
       <c r="H40" s="30"/>
       <c r="I40" s="30"/>
@@ -4358,7 +4439,7 @@
       <c r="K40" s="17"/>
       <c r="L40" s="25"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>28</v>
       </c>
@@ -4375,7 +4456,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F43" s="31"/>
       <c r="H43" s="30"/>
       <c r="I43" s="30"/>
@@ -4383,7 +4464,7 @@
       <c r="K43" s="17"/>
       <c r="L43" s="25"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="26"/>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
@@ -4398,27 +4479,19 @@
       <c r="L44" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
+  <mergeCells count="48">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="A15:A17"/>
@@ -4435,17 +4508,26 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <conditionalFormatting sqref="L15:L39 I33:J33">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
@@ -4474,27 +4556,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:L7"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="68" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="68"/>
-    <col min="4" max="4" width="2.7109375" style="68" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" style="68" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="68" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" style="68" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" style="68" customWidth="1"/>
-    <col min="10" max="11" width="7.28515625" style="68" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="68" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="68" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="68"/>
+    <col min="1" max="1" width="7.265625" style="68" customWidth="1"/>
+    <col min="2" max="3" width="9.1328125" style="68"/>
+    <col min="4" max="4" width="2.73046875" style="68" customWidth="1"/>
+    <col min="5" max="6" width="7.265625" style="68" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" style="68" customWidth="1"/>
+    <col min="8" max="8" width="4.86328125" style="68" customWidth="1"/>
+    <col min="9" max="9" width="2.86328125" style="68" customWidth="1"/>
+    <col min="10" max="11" width="7.265625" style="68" customWidth="1"/>
+    <col min="12" max="12" width="9.1328125" style="68" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="68" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="106" t="s">
         <v>77</v>
       </c>
@@ -4506,7 +4588,7 @@
       <c r="K2" s="99"/>
       <c r="L2" s="99"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="105" t="s">
         <v>78</v>
       </c>
@@ -4518,14 +4600,14 @@
       <c r="K3" s="99"/>
       <c r="L3" s="99"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="75"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="C4" s="270"/>
+      <c r="D4" s="270"/>
+      <c r="E4" s="270"/>
       <c r="F4" s="104"/>
       <c r="H4" s="102"/>
       <c r="I4" s="101" t="s">
@@ -4535,15 +4617,15 @@
       <c r="K4" s="99"/>
       <c r="L4" s="99"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="87" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="87"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
+      <c r="C5" s="269"/>
+      <c r="D5" s="269"/>
+      <c r="E5" s="269"/>
+      <c r="F5" s="269"/>
       <c r="H5" s="102"/>
       <c r="I5" s="101" t="s">
         <v>13</v>
@@ -4552,18 +4634,18 @@
       <c r="K5" s="99"/>
       <c r="L5" s="99"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="87"/>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
+      <c r="C6" s="269"/>
+      <c r="D6" s="269"/>
+      <c r="E6" s="269"/>
+      <c r="F6" s="269"/>
       <c r="K6" s="98"/>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="87" t="s">
         <v>69</v>
       </c>
@@ -4580,66 +4662,66 @@
       <c r="K7" s="96"/>
       <c r="L7" s="95"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="75" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="75"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
+      <c r="C8" s="270"/>
+      <c r="D8" s="270"/>
+      <c r="E8" s="270"/>
+      <c r="F8" s="270"/>
       <c r="H8" s="94"/>
       <c r="I8" s="94"/>
       <c r="J8" s="94"/>
       <c r="K8" s="94"/>
       <c r="L8" s="94"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="87"/>
-      <c r="C9" s="284"/>
-      <c r="D9" s="284"/>
-      <c r="E9" s="284"/>
-      <c r="F9" s="284"/>
+      <c r="C9" s="269"/>
+      <c r="D9" s="269"/>
+      <c r="E9" s="269"/>
+      <c r="F9" s="269"/>
       <c r="H9" s="94"/>
       <c r="I9" s="94"/>
       <c r="J9" s="94"/>
       <c r="K9" s="94"/>
       <c r="L9" s="94"/>
     </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="87" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="87"/>
-      <c r="C10" s="284"/>
-      <c r="D10" s="284"/>
-      <c r="E10" s="284"/>
-      <c r="F10" s="284"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
       <c r="H10" s="94"/>
       <c r="I10" s="94"/>
       <c r="J10" s="94"/>
       <c r="K10" s="94"/>
       <c r="L10" s="94"/>
     </row>
-    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="94"/>
       <c r="I11" s="94"/>
       <c r="J11" s="94"/>
       <c r="K11" s="94"/>
       <c r="L11" s="94"/>
     </row>
-    <row r="12" spans="1:13" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="94"/>
       <c r="I12" s="94"/>
       <c r="J12" s="94"/>
       <c r="K12" s="94"/>
       <c r="L12" s="94"/>
     </row>
-    <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="93"/>
       <c r="B13" s="87"/>
       <c r="C13" s="92"/>
@@ -4658,7 +4740,7 @@
       </c>
       <c r="M13" s="74"/>
     </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="126" t="s">
         <v>25</v>
       </c>
@@ -4674,7 +4756,7 @@
       <c r="K14" s="90"/>
       <c r="L14" s="84"/>
     </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="126" t="s">
         <v>33</v>
       </c>
@@ -4690,7 +4772,7 @@
       <c r="K15" s="86"/>
       <c r="L15" s="84"/>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="126" t="s">
         <v>79</v>
       </c>
@@ -4706,7 +4788,7 @@
       <c r="K16" s="86"/>
       <c r="L16" s="84"/>
     </row>
-    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="126" t="s">
         <v>70</v>
       </c>
@@ -4722,7 +4804,7 @@
       <c r="K17" s="86"/>
       <c r="L17" s="84"/>
     </row>
-    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="129" t="s">
         <v>35</v>
       </c>
@@ -4738,7 +4820,7 @@
       <c r="K18" s="86"/>
       <c r="L18" s="84"/>
     </row>
-    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="129" t="s">
         <v>36</v>
       </c>
@@ -4754,11 +4836,11 @@
       <c r="K19" s="86"/>
       <c r="L19" s="84"/>
     </row>
-    <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K20" s="85"/>
       <c r="L20" s="85"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="74"/>
       <c r="C21" s="74"/>
       <c r="D21" s="74"/>
@@ -4774,7 +4856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
       <c r="D22" s="74"/>
@@ -4783,7 +4865,7 @@
       <c r="I22" s="70"/>
       <c r="J22" s="81"/>
     </row>
-    <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="47" t="s">
         <v>3</v>
       </c>
@@ -4792,96 +4874,96 @@
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
-      <c r="G23" s="269" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="270"/>
-      <c r="I23" s="271"/>
+      <c r="G23" s="274" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="275"/>
+      <c r="I23" s="276"/>
       <c r="J23" s="197" t="s">
         <v>7</v>
       </c>
       <c r="K23" s="198"/>
       <c r="L23" s="199"/>
     </row>
-    <row r="24" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="200" t="s">
+    <row r="24" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="203" t="s">
+      <c r="B24" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="203" t="s">
+      <c r="C24" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="203"/>
-      <c r="E24" s="205" t="s">
+      <c r="D24" s="201"/>
+      <c r="E24" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="281"/>
-      <c r="G24" s="272"/>
-      <c r="H24" s="273"/>
-      <c r="I24" s="274"/>
-      <c r="J24" s="209">
+      <c r="F24" s="271"/>
+      <c r="G24" s="277"/>
+      <c r="H24" s="278"/>
+      <c r="I24" s="279"/>
+      <c r="J24" s="207">
         <v>0.2</v>
       </c>
-      <c r="K24" s="212"/>
-      <c r="L24" s="215">
+      <c r="K24" s="210"/>
+      <c r="L24" s="213">
         <f>K24*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="201"/>
-      <c r="B25" s="203"/>
-      <c r="C25" s="203" t="s">
+    <row r="25" spans="1:13" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="200"/>
+      <c r="B25" s="201"/>
+      <c r="C25" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="203"/>
-      <c r="E25" s="216" t="s">
+      <c r="D25" s="201"/>
+      <c r="E25" s="214" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="217"/>
-      <c r="G25" s="275"/>
-      <c r="H25" s="276"/>
-      <c r="I25" s="277"/>
-      <c r="J25" s="210"/>
-      <c r="K25" s="212"/>
-      <c r="L25" s="282"/>
-    </row>
-    <row r="26" spans="1:13" s="11" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="202"/>
-      <c r="B26" s="204"/>
-      <c r="C26" s="204" t="s">
+      <c r="F25" s="215"/>
+      <c r="G25" s="280"/>
+      <c r="H25" s="281"/>
+      <c r="I25" s="282"/>
+      <c r="J25" s="208"/>
+      <c r="K25" s="210"/>
+      <c r="L25" s="272"/>
+    </row>
+    <row r="26" spans="1:13" s="11" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="184"/>
+      <c r="B26" s="202"/>
+      <c r="C26" s="202" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="204"/>
-      <c r="E26" s="216" t="s">
+      <c r="D26" s="202"/>
+      <c r="E26" s="214" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="217"/>
-      <c r="G26" s="275"/>
-      <c r="H26" s="276"/>
-      <c r="I26" s="277"/>
-      <c r="J26" s="211"/>
-      <c r="K26" s="213"/>
-      <c r="L26" s="283"/>
-    </row>
-    <row r="27" spans="1:13" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="200" t="s">
+      <c r="F26" s="215"/>
+      <c r="G26" s="280"/>
+      <c r="H26" s="281"/>
+      <c r="I26" s="282"/>
+      <c r="J26" s="209"/>
+      <c r="K26" s="211"/>
+      <c r="L26" s="273"/>
+    </row>
+    <row r="27" spans="1:13" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="225" t="s">
+      <c r="B27" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="226"/>
-      <c r="D27" s="227"/>
-      <c r="E27" s="228" t="s">
+      <c r="C27" s="186"/>
+      <c r="D27" s="187"/>
+      <c r="E27" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="229"/>
-      <c r="G27" s="278"/>
-      <c r="H27" s="279"/>
-      <c r="I27" s="280"/>
+      <c r="F27" s="189"/>
+      <c r="G27" s="283"/>
+      <c r="H27" s="284"/>
+      <c r="I27" s="285"/>
       <c r="J27" s="66">
         <v>0.4</v>
       </c>
@@ -4892,20 +4974,20 @@
       </c>
       <c r="M27" s="26"/>
     </row>
-    <row r="28" spans="1:13" s="11" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="202"/>
-      <c r="B28" s="230" t="s">
+    <row r="28" spans="1:13" s="11" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="184"/>
+      <c r="B28" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="231"/>
-      <c r="D28" s="232"/>
-      <c r="E28" s="233" t="s">
+      <c r="C28" s="193"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="234"/>
-      <c r="G28" s="275"/>
-      <c r="H28" s="276"/>
-      <c r="I28" s="277"/>
+      <c r="F28" s="196"/>
+      <c r="G28" s="280"/>
+      <c r="H28" s="281"/>
+      <c r="I28" s="282"/>
       <c r="J28" s="66">
         <v>0.4</v>
       </c>
@@ -4915,20 +4997,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="11" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="11" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="222" t="s">
+      <c r="B29" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="223"/>
-      <c r="D29" s="223"/>
-      <c r="E29" s="223"/>
-      <c r="F29" s="223"/>
-      <c r="G29" s="223"/>
-      <c r="H29" s="223"/>
-      <c r="I29" s="224"/>
+      <c r="C29" s="181"/>
+      <c r="D29" s="181"/>
+      <c r="E29" s="181"/>
+      <c r="F29" s="181"/>
+      <c r="G29" s="181"/>
+      <c r="H29" s="181"/>
+      <c r="I29" s="182"/>
       <c r="J29" s="67"/>
       <c r="K29" s="61">
         <f>J29</f>
@@ -4936,7 +5018,7 @@
       </c>
       <c r="L29" s="140"/>
     </row>
-    <row r="30" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="52"/>
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
@@ -4954,7 +5036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="52"/>
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
@@ -4972,7 +5054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="52"/>
       <c r="B32" s="52"/>
       <c r="C32" s="52"/>
@@ -4990,7 +5072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="77" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="77" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I33" s="80"/>
       <c r="J33" s="79" t="s">
         <v>71</v>
@@ -5001,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="74"/>
       <c r="C34" s="74"/>
       <c r="D34" s="74"/>
@@ -5013,7 +5095,7 @@
       <c r="K34" s="70"/>
       <c r="L34" s="69"/>
     </row>
-    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="75" t="s">
         <v>28</v>
       </c>
@@ -5031,7 +5113,7 @@
       <c r="K35" s="75"/>
       <c r="L35" s="75"/>
     </row>
-    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="74"/>
       <c r="C36" s="74"/>
       <c r="D36" s="74"/>
@@ -5044,12 +5126,20 @@
       <c r="L36" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C6:F6"/>
+  <mergeCells count="30">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
@@ -5062,18 +5152,11 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="L24 L27:L28 K29 L30:L32">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
@@ -5099,28 +5182,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="110" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="110" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="110" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="110" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" style="110" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="110" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="110" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="110" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="110" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="110" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" style="110" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="110"/>
+    <col min="1" max="1" width="11.86328125" style="110" customWidth="1"/>
+    <col min="2" max="2" width="7.3984375" style="110" customWidth="1"/>
+    <col min="3" max="3" width="7.86328125" style="110" customWidth="1"/>
+    <col min="4" max="4" width="6.3984375" style="110" customWidth="1"/>
+    <col min="5" max="6" width="7.265625" style="110" customWidth="1"/>
+    <col min="7" max="7" width="7.73046875" style="110" customWidth="1"/>
+    <col min="8" max="8" width="6.1328125" style="110" customWidth="1"/>
+    <col min="9" max="9" width="7.265625" style="110" customWidth="1"/>
+    <col min="10" max="10" width="6.59765625" style="110" customWidth="1"/>
+    <col min="11" max="11" width="8.3984375" style="110" customWidth="1"/>
+    <col min="12" max="12" width="6.3984375" style="110" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="110"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="119" t="s">
         <v>81</v>
       </c>
@@ -5132,7 +5215,7 @@
       <c r="K2" s="176"/>
       <c r="L2" s="174"/>
     </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="116" t="s">
         <v>57</v>
       </c>
@@ -5144,14 +5227,14 @@
       <c r="K3" s="176"/>
       <c r="L3" s="174"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="111" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="111"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
+      <c r="C4" s="293"/>
+      <c r="D4" s="293"/>
+      <c r="E4" s="293"/>
       <c r="F4" s="118"/>
       <c r="H4" s="79" t="s">
         <v>11</v>
@@ -5161,15 +5244,15 @@
       <c r="K4" s="176"/>
       <c r="L4" s="174"/>
     </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="115" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="115"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
+      <c r="C5" s="292"/>
+      <c r="D5" s="292"/>
+      <c r="E5" s="292"/>
+      <c r="F5" s="292"/>
       <c r="H5" s="79" t="s">
         <v>13</v>
       </c>
@@ -5178,22 +5261,22 @@
       <c r="K5" s="176"/>
       <c r="L5" s="174"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="115" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="115"/>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286"/>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
+      <c r="C6" s="292"/>
+      <c r="D6" s="292"/>
+      <c r="E6" s="292"/>
+      <c r="F6" s="292"/>
       <c r="H6" s="68"/>
       <c r="I6" s="68"/>
       <c r="J6" s="68"/>
       <c r="K6" s="98"/>
       <c r="L6" s="74"/>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="115" t="s">
         <v>69</v>
       </c>
@@ -5210,59 +5293,59 @@
       <c r="K7" s="178"/>
       <c r="L7" s="175"/>
     </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="111" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="111"/>
-      <c r="C8" s="287"/>
-      <c r="D8" s="287"/>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
+      <c r="C8" s="293"/>
+      <c r="D8" s="293"/>
+      <c r="E8" s="293"/>
+      <c r="F8" s="293"/>
       <c r="H8" s="117"/>
       <c r="I8" s="117"/>
       <c r="J8" s="117"/>
       <c r="K8" s="117"/>
       <c r="L8" s="117"/>
     </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="115" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="115"/>
-      <c r="C9" s="286"/>
-      <c r="D9" s="286"/>
-      <c r="E9" s="286"/>
-      <c r="F9" s="286"/>
+      <c r="C9" s="292"/>
+      <c r="D9" s="292"/>
+      <c r="E9" s="292"/>
+      <c r="F9" s="292"/>
       <c r="H9" s="117"/>
       <c r="I9" s="117"/>
       <c r="J9" s="117"/>
       <c r="K9" s="117"/>
       <c r="L9" s="117"/>
     </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="115" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="286"/>
-      <c r="D10" s="286"/>
-      <c r="E10" s="286"/>
-      <c r="F10" s="286"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
       <c r="H10" s="117"/>
       <c r="I10" s="117"/>
       <c r="J10" s="117"/>
       <c r="K10" s="117"/>
       <c r="L10" s="117"/>
     </row>
-    <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="117"/>
       <c r="I11" s="117"/>
       <c r="J11" s="117"/>
       <c r="K11" s="117"/>
       <c r="L11" s="117"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="114"/>
       <c r="B12" s="114"/>
       <c r="C12" s="114"/>
@@ -5276,7 +5359,7 @@
       <c r="K12" s="113"/>
       <c r="L12" s="114"/>
     </row>
-    <row r="13" spans="1:12" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="11" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
         <v>3</v>
       </c>
@@ -5285,147 +5368,147 @@
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="48"/>
-      <c r="G13" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="196"/>
+      <c r="G13" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="225"/>
       <c r="I13" s="197" t="s">
         <v>7</v>
       </c>
       <c r="J13" s="198"/>
       <c r="K13" s="199"/>
     </row>
-    <row r="14" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="250" t="s">
+    <row r="14" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="235" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="263" t="s">
+      <c r="B14" s="238" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="263" t="s">
+      <c r="C14" s="238" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="263"/>
-      <c r="E14" s="255" t="s">
+      <c r="D14" s="238"/>
+      <c r="E14" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="265"/>
-      <c r="G14" s="207"/>
-      <c r="H14" s="208"/>
-      <c r="I14" s="209">
+      <c r="F14" s="241"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="206"/>
+      <c r="I14" s="207">
         <v>0.2</v>
       </c>
-      <c r="J14" s="212">
+      <c r="J14" s="210">
+        <v>0</v>
+      </c>
+      <c r="K14" s="212">
+        <f>J14*0.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="236"/>
+      <c r="B15" s="238"/>
+      <c r="C15" s="238" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="238"/>
+      <c r="E15" s="242" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="243"/>
+      <c r="G15" s="190"/>
+      <c r="H15" s="191"/>
+      <c r="I15" s="208"/>
+      <c r="J15" s="210"/>
+      <c r="K15" s="212"/>
+    </row>
+    <row r="16" spans="1:12" s="11" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="237"/>
+      <c r="B16" s="239"/>
+      <c r="C16" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="214">
-        <f>J14*0.2</f>
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="262"/>
-      <c r="B15" s="263"/>
-      <c r="C15" s="263" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="263"/>
-      <c r="E15" s="266" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="267"/>
-      <c r="G15" s="218"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="210"/>
-      <c r="J15" s="212"/>
-      <c r="K15" s="214"/>
-    </row>
-    <row r="16" spans="1:12" s="11" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="251"/>
-      <c r="B16" s="264"/>
-      <c r="C16" s="264" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="264"/>
-      <c r="E16" s="266" t="s">
+      <c r="D16" s="239"/>
+      <c r="E16" s="242" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="267"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="221"/>
-      <c r="I16" s="211"/>
-      <c r="J16" s="213"/>
-      <c r="K16" s="215"/>
-    </row>
-    <row r="17" spans="1:12" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="250" t="s">
+      <c r="F16" s="243"/>
+      <c r="G16" s="216"/>
+      <c r="H16" s="217"/>
+      <c r="I16" s="209"/>
+      <c r="J16" s="211"/>
+      <c r="K16" s="213"/>
+    </row>
+    <row r="17" spans="1:12" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="252" t="s">
+      <c r="B17" s="244" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="253"/>
-      <c r="D17" s="254"/>
-      <c r="E17" s="255" t="s">
+      <c r="C17" s="245"/>
+      <c r="D17" s="246"/>
+      <c r="E17" s="240" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="256"/>
-      <c r="G17" s="218"/>
-      <c r="H17" s="219"/>
+      <c r="F17" s="247"/>
+      <c r="G17" s="190"/>
+      <c r="H17" s="191"/>
       <c r="I17" s="49">
         <v>0.4</v>
       </c>
       <c r="J17" s="151">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K17" s="152">
         <f>J17*0.4</f>
-        <v>2.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="L17" s="26"/>
     </row>
-    <row r="18" spans="1:12" s="11" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="251"/>
-      <c r="B18" s="257" t="s">
+    <row r="18" spans="1:12" s="11" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="237"/>
+      <c r="B18" s="248" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="258"/>
-      <c r="D18" s="259"/>
-      <c r="E18" s="260" t="s">
+      <c r="C18" s="249"/>
+      <c r="D18" s="250"/>
+      <c r="E18" s="251" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="261"/>
-      <c r="G18" s="218"/>
-      <c r="H18" s="219"/>
+      <c r="F18" s="252"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="191"/>
       <c r="I18" s="49">
         <v>0.4</v>
       </c>
       <c r="J18" s="151">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K18" s="152">
         <f>J18*0.4</f>
-        <v>2.4000000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="11" customFormat="1" ht="13.15" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="222" t="s">
+      <c r="B19" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="223"/>
-      <c r="D19" s="223"/>
-      <c r="E19" s="223"/>
-      <c r="F19" s="223"/>
-      <c r="G19" s="223"/>
-      <c r="H19" s="223"/>
-      <c r="I19" s="224"/>
+      <c r="C19" s="181"/>
+      <c r="D19" s="181"/>
+      <c r="E19" s="181"/>
+      <c r="F19" s="181"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="181"/>
+      <c r="I19" s="182"/>
       <c r="J19" s="50"/>
       <c r="K19" s="155"/>
     </row>
-    <row r="20" spans="1:12" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="52"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52"/>
@@ -5438,10 +5521,10 @@
       <c r="J20" s="33"/>
       <c r="K20" s="53">
         <f>(K14+K17+K18)-K19</f>
-        <v>6.0000000000000009</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="54" t="s">
         <v>57</v>
       </c>
@@ -5458,7 +5541,7 @@
       <c r="J21" s="33"/>
       <c r="K21" s="36"/>
     </row>
-    <row r="22" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="52"/>
       <c r="B22" s="46">
         <v>1</v>
@@ -5482,34 +5565,34 @@
       <c r="I22" s="33"/>
       <c r="J22" s="36"/>
     </row>
-    <row r="23" spans="1:12" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="55" t="s">
         <v>82</v>
       </c>
       <c r="B23" s="141">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C23" s="141">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D23" s="141">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E23" s="141">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F23" s="141">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G23" s="142">
         <f>IFERROR(B23+C23+D23+E23+F23,0)</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
       <c r="J23" s="36"/>
     </row>
-    <row r="24" spans="1:12" s="11" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="11" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="52"/>
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
@@ -5522,13 +5605,13 @@
       </c>
       <c r="G24" s="143">
         <f>G23/5</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="J24" s="36"/>
     </row>
-    <row r="25" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
       <c r="D25" s="52"/>
@@ -5540,121 +5623,121 @@
       <c r="J25" s="33"/>
       <c r="K25" s="33"/>
     </row>
-    <row r="26" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="240" t="s">
+    <row r="26" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="241"/>
-      <c r="C26" s="241"/>
-      <c r="D26" s="241"/>
-      <c r="E26" s="241"/>
-      <c r="F26" s="241"/>
-      <c r="G26" s="241"/>
-      <c r="H26" s="241"/>
-      <c r="I26" s="241"/>
-      <c r="J26" s="241"/>
-      <c r="K26" s="242"/>
-    </row>
-    <row r="27" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="243"/>
-      <c r="B27" s="244"/>
-      <c r="C27" s="244"/>
-      <c r="D27" s="244"/>
-      <c r="E27" s="244"/>
-      <c r="F27" s="244"/>
-      <c r="G27" s="244"/>
-      <c r="H27" s="244"/>
-      <c r="I27" s="244"/>
-      <c r="J27" s="244"/>
-      <c r="K27" s="245"/>
-    </row>
-    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="243"/>
-      <c r="B28" s="244"/>
-      <c r="C28" s="244"/>
-      <c r="D28" s="244"/>
-      <c r="E28" s="244"/>
-      <c r="F28" s="244"/>
-      <c r="G28" s="244"/>
-      <c r="H28" s="244"/>
-      <c r="I28" s="244"/>
-      <c r="J28" s="244"/>
-      <c r="K28" s="245"/>
-    </row>
-    <row r="29" spans="1:12" s="11" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="243"/>
-      <c r="B29" s="244"/>
-      <c r="C29" s="244"/>
-      <c r="D29" s="244"/>
-      <c r="E29" s="244"/>
-      <c r="F29" s="244"/>
-      <c r="G29" s="244"/>
-      <c r="H29" s="244"/>
-      <c r="I29" s="244"/>
-      <c r="J29" s="244"/>
-      <c r="K29" s="245"/>
-    </row>
-    <row r="30" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="246"/>
-      <c r="B30" s="247"/>
-      <c r="C30" s="247"/>
-      <c r="D30" s="247"/>
-      <c r="E30" s="247"/>
-      <c r="F30" s="247"/>
-      <c r="G30" s="247"/>
-      <c r="H30" s="247"/>
-      <c r="I30" s="247"/>
-      <c r="J30" s="247"/>
-      <c r="K30" s="248"/>
-    </row>
-    <row r="31" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:12" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="291" t="s">
+      <c r="B26" s="259"/>
+      <c r="C26" s="259"/>
+      <c r="D26" s="259"/>
+      <c r="E26" s="259"/>
+      <c r="F26" s="259"/>
+      <c r="G26" s="259"/>
+      <c r="H26" s="259"/>
+      <c r="I26" s="259"/>
+      <c r="J26" s="259"/>
+      <c r="K26" s="260"/>
+    </row>
+    <row r="27" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="261"/>
+      <c r="B27" s="262"/>
+      <c r="C27" s="262"/>
+      <c r="D27" s="262"/>
+      <c r="E27" s="262"/>
+      <c r="F27" s="262"/>
+      <c r="G27" s="262"/>
+      <c r="H27" s="262"/>
+      <c r="I27" s="262"/>
+      <c r="J27" s="262"/>
+      <c r="K27" s="263"/>
+    </row>
+    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="261"/>
+      <c r="B28" s="262"/>
+      <c r="C28" s="262"/>
+      <c r="D28" s="262"/>
+      <c r="E28" s="262"/>
+      <c r="F28" s="262"/>
+      <c r="G28" s="262"/>
+      <c r="H28" s="262"/>
+      <c r="I28" s="262"/>
+      <c r="J28" s="262"/>
+      <c r="K28" s="263"/>
+    </row>
+    <row r="29" spans="1:12" s="11" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="261"/>
+      <c r="B29" s="262"/>
+      <c r="C29" s="262"/>
+      <c r="D29" s="262"/>
+      <c r="E29" s="262"/>
+      <c r="F29" s="262"/>
+      <c r="G29" s="262"/>
+      <c r="H29" s="262"/>
+      <c r="I29" s="262"/>
+      <c r="J29" s="262"/>
+      <c r="K29" s="263"/>
+    </row>
+    <row r="30" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="264"/>
+      <c r="B30" s="265"/>
+      <c r="C30" s="265"/>
+      <c r="D30" s="265"/>
+      <c r="E30" s="265"/>
+      <c r="F30" s="265"/>
+      <c r="G30" s="265"/>
+      <c r="H30" s="265"/>
+      <c r="I30" s="265"/>
+      <c r="J30" s="265"/>
+      <c r="K30" s="266"/>
+    </row>
+    <row r="31" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="289" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="291"/>
-      <c r="C32" s="291"/>
-      <c r="D32" s="291"/>
-      <c r="E32" s="291"/>
-      <c r="F32" s="291"/>
-      <c r="G32" s="291"/>
-      <c r="H32" s="293">
+      <c r="B32" s="289"/>
+      <c r="C32" s="289"/>
+      <c r="D32" s="289"/>
+      <c r="E32" s="289"/>
+      <c r="F32" s="289"/>
+      <c r="G32" s="289"/>
+      <c r="H32" s="291">
         <f>G24</f>
-        <v>6</v>
-      </c>
-      <c r="I32" s="293"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="291"/>
       <c r="J32" s="165" t="s">
         <v>47</v>
       </c>
       <c r="K32" s="153">
         <f>H32*3</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="291" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="289" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="291"/>
-      <c r="C33" s="291"/>
-      <c r="D33" s="291"/>
-      <c r="E33" s="291"/>
-      <c r="F33" s="291"/>
-      <c r="G33" s="291"/>
-      <c r="H33" s="249">
+      <c r="B33" s="289"/>
+      <c r="C33" s="289"/>
+      <c r="D33" s="289"/>
+      <c r="E33" s="289"/>
+      <c r="F33" s="289"/>
+      <c r="G33" s="289"/>
+      <c r="H33" s="267">
         <f>K20</f>
-        <v>6.0000000000000009</v>
-      </c>
-      <c r="I33" s="292"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="290"/>
       <c r="J33" s="166" t="s">
         <v>63</v>
       </c>
       <c r="K33" s="153">
         <f>H33</f>
-        <v>6.0000000000000009</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="11" customFormat="1" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="167"/>
       <c r="B34" s="168"/>
       <c r="C34" s="168"/>
@@ -5669,28 +5752,28 @@
       </c>
       <c r="K34" s="153">
         <f>(K32+K33)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="11" customFormat="1" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="167"/>
       <c r="B35" s="167"/>
       <c r="C35" s="167"/>
       <c r="D35" s="167"/>
-      <c r="E35" s="288" t="s">
+      <c r="E35" s="286" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="289"/>
-      <c r="G35" s="289"/>
-      <c r="H35" s="289"/>
-      <c r="I35" s="289"/>
-      <c r="J35" s="290"/>
+      <c r="F35" s="287"/>
+      <c r="G35" s="287"/>
+      <c r="H35" s="287"/>
+      <c r="I35" s="287"/>
+      <c r="J35" s="288"/>
       <c r="K35" s="58">
         <f>K34/4</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A36" s="167"/>
       <c r="B36" s="167"/>
       <c r="C36" s="167"/>
@@ -5703,7 +5786,7 @@
       <c r="J36" s="173"/>
       <c r="K36" s="145"/>
     </row>
-    <row r="37" spans="1:12" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A37" s="52"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
@@ -5716,7 +5799,7 @@
       <c r="J37" s="28"/>
       <c r="K37" s="59"/>
     </row>
-    <row r="38" spans="1:12" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A38" s="52"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
@@ -5729,7 +5812,7 @@
       <c r="J38" s="28"/>
       <c r="K38" s="59"/>
     </row>
-    <row r="39" spans="1:12" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A39" s="52"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
@@ -5742,7 +5825,7 @@
       <c r="J39" s="28"/>
       <c r="K39" s="59"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="114"/>
       <c r="B40" s="114"/>
       <c r="C40" s="114"/>
@@ -5756,7 +5839,7 @@
       <c r="K40" s="59"/>
       <c r="L40" s="114"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="111" t="s">
         <v>28</v>
       </c>
@@ -5774,26 +5857,8 @@
       <c r="L41" s="111"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="A26:K30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+  <mergeCells count="36">
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="A14:A16"/>
@@ -5810,6 +5875,25 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="A26:K30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="H32:I32"/>
   </mergeCells>
   <conditionalFormatting sqref="H33:I33 K14:K21 J22:J24 K25:K40">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>

<commit_message>
Nya protokoll och justering armnr
</commit_message>
<xml_diff>
--- a/mallar/Protokoll 2017 lättklass lag o ind_justerad.xlsx
+++ b/mallar/Protokoll 2017 lättklass lag o ind_justerad.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="muK/Rsgn0FngGE/mV/SY/MPxEFarFdZF3g0P1PGbjFCV9x5F8AG9QOlpeVa8cMCwcnfLIvLNCjpGfdHDMXsAuQ==" workbookSaltValue="s+AIShC46YCzrqNSDCe49g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="15120" windowHeight="7410" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="15120" windowHeight="7410" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="8" r:id="rId1"/>
@@ -1431,6 +1431,146 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1447,15 +1587,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1466,135 +1597,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,12 +1669,6 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1657,9 +1678,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
@@ -1676,30 +1694,21 @@
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1739,41 +1748,32 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2229,7 +2229,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2370,9 +2370,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A37" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
@@ -2415,8 +2418,8 @@
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="180"/>
-      <c r="D4" s="180"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42"/>
       <c r="G4" s="3"/>
       <c r="H4" s="7" t="s">
@@ -2431,9 +2434,9 @@
         <v>12</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="232"/>
       <c r="G5" s="3"/>
       <c r="H5" s="7" t="s">
         <v>13</v>
@@ -2455,83 +2458,83 @@
         <v>15</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="189"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
+      <c r="C7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
       <c r="G7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="191"/>
-      <c r="I7" s="192"/>
-      <c r="J7" s="192"/>
-      <c r="K7" s="192"/>
+      <c r="H7" s="234"/>
+      <c r="I7" s="235"/>
+      <c r="J7" s="235"/>
+      <c r="K7" s="235"/>
     </row>
     <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="190"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="190"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
       <c r="G8" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="181"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="228"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="228"/>
     </row>
     <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="232"/>
       <c r="G9" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="181"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="182"/>
+      <c r="H9" s="227"/>
+      <c r="I9" s="228"/>
+      <c r="J9" s="228"/>
+      <c r="K9" s="228"/>
     </row>
     <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
       <c r="G10" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="181"/>
-      <c r="I10" s="182"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="182"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="228"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="228"/>
     </row>
     <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="181"/>
-      <c r="I11" s="182"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="182"/>
+      <c r="H11" s="227"/>
+      <c r="I11" s="228"/>
+      <c r="J11" s="228"/>
+      <c r="K11" s="228"/>
     </row>
     <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="G12" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="181"/>
-      <c r="I12" s="182"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="182"/>
+      <c r="H12" s="227"/>
+      <c r="I12" s="228"/>
+      <c r="J12" s="228"/>
+      <c r="K12" s="228"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
@@ -2561,11 +2564,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="183" t="s">
+      <c r="A15" s="229" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="184"/>
-      <c r="C15" s="185"/>
+      <c r="B15" s="230"/>
+      <c r="C15" s="231"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -2578,11 +2581,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="186" t="s">
+      <c r="A16" s="218" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="187"/>
-      <c r="C16" s="188"/>
+      <c r="B16" s="219"/>
+      <c r="C16" s="220"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -2595,11 +2598,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="186" t="s">
+      <c r="A17" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="187"/>
-      <c r="C17" s="188"/>
+      <c r="B17" s="219"/>
+      <c r="C17" s="220"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -2612,11 +2615,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="193" t="s">
+      <c r="A18" s="221" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="194"/>
-      <c r="C18" s="195"/>
+      <c r="B18" s="222"/>
+      <c r="C18" s="223"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -2629,11 +2632,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="186" t="s">
+      <c r="A19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="187"/>
-      <c r="C19" s="188"/>
+      <c r="B19" s="219"/>
+      <c r="C19" s="220"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -2646,11 +2649,11 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="186" t="s">
+      <c r="A20" s="218" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="187"/>
-      <c r="C20" s="188"/>
+      <c r="B20" s="219"/>
+      <c r="C20" s="220"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -2739,91 +2742,91 @@
       <c r="D28" s="48"/>
       <c r="E28" s="48"/>
       <c r="F28" s="48"/>
-      <c r="G28" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="197"/>
-      <c r="I28" s="198" t="s">
+      <c r="G28" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="225"/>
+      <c r="I28" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="J28" s="199"/>
-      <c r="K28" s="200"/>
+      <c r="J28" s="198"/>
+      <c r="K28" s="199"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="201" t="s">
+      <c r="A29" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="204" t="s">
+      <c r="B29" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="204" t="s">
+      <c r="C29" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="204"/>
-      <c r="E29" s="206" t="s">
+      <c r="D29" s="201"/>
+      <c r="E29" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="207"/>
-      <c r="G29" s="208"/>
-      <c r="H29" s="209"/>
-      <c r="I29" s="210">
+      <c r="F29" s="204"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="206"/>
+      <c r="I29" s="207">
         <v>0.2</v>
       </c>
-      <c r="J29" s="213"/>
-      <c r="K29" s="215">
+      <c r="J29" s="210"/>
+      <c r="K29" s="212">
         <f>J29*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="202"/>
-      <c r="B30" s="204"/>
-      <c r="C30" s="204" t="s">
+      <c r="A30" s="200"/>
+      <c r="B30" s="201"/>
+      <c r="C30" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="204"/>
-      <c r="E30" s="217" t="s">
+      <c r="D30" s="201"/>
+      <c r="E30" s="214" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="218"/>
-      <c r="G30" s="219"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="211"/>
-      <c r="J30" s="213"/>
-      <c r="K30" s="215"/>
+      <c r="F30" s="215"/>
+      <c r="G30" s="190"/>
+      <c r="H30" s="191"/>
+      <c r="I30" s="208"/>
+      <c r="J30" s="210"/>
+      <c r="K30" s="212"/>
     </row>
     <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="203"/>
-      <c r="B31" s="205"/>
-      <c r="C31" s="205" t="s">
+      <c r="A31" s="184"/>
+      <c r="B31" s="202"/>
+      <c r="C31" s="202" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="205"/>
-      <c r="E31" s="217" t="s">
+      <c r="D31" s="202"/>
+      <c r="E31" s="214" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="218"/>
-      <c r="G31" s="221"/>
-      <c r="H31" s="222"/>
-      <c r="I31" s="212"/>
-      <c r="J31" s="214"/>
-      <c r="K31" s="216"/>
+      <c r="F31" s="215"/>
+      <c r="G31" s="216"/>
+      <c r="H31" s="217"/>
+      <c r="I31" s="209"/>
+      <c r="J31" s="211"/>
+      <c r="K31" s="213"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="201" t="s">
+      <c r="A32" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="226" t="s">
+      <c r="B32" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="227"/>
-      <c r="D32" s="228"/>
-      <c r="E32" s="229" t="s">
+      <c r="C32" s="186"/>
+      <c r="D32" s="187"/>
+      <c r="E32" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="230"/>
-      <c r="G32" s="219"/>
-      <c r="H32" s="220"/>
+      <c r="F32" s="189"/>
+      <c r="G32" s="190"/>
+      <c r="H32" s="191"/>
       <c r="I32" s="49">
         <v>0.4</v>
       </c>
@@ -2834,18 +2837,18 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="203"/>
-      <c r="B33" s="231" t="s">
+      <c r="A33" s="184"/>
+      <c r="B33" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="232"/>
-      <c r="D33" s="233"/>
-      <c r="E33" s="234" t="s">
+      <c r="C33" s="193"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="195" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="235"/>
-      <c r="G33" s="219"/>
-      <c r="H33" s="220"/>
+      <c r="F33" s="196"/>
+      <c r="G33" s="190"/>
+      <c r="H33" s="191"/>
       <c r="I33" s="49">
         <v>0.4</v>
       </c>
@@ -2859,16 +2862,16 @@
       <c r="A34" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="223" t="s">
+      <c r="B34" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="224"/>
-      <c r="D34" s="224"/>
-      <c r="E34" s="224"/>
-      <c r="F34" s="224"/>
-      <c r="G34" s="224"/>
-      <c r="H34" s="224"/>
-      <c r="I34" s="225"/>
+      <c r="C34" s="181"/>
+      <c r="D34" s="181"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="181"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="181"/>
+      <c r="I34" s="182"/>
       <c r="J34" s="60"/>
       <c r="K34" s="154">
         <f>J34</f>
@@ -2973,14 +2976,25 @@
     <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="B29:B31"/>
@@ -2996,25 +3010,14 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
   </mergeCells>
   <conditionalFormatting sqref="K29:K37">
     <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
@@ -3028,7 +3031,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="97" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LÄTTKLASS</oddHeader>
   </headerFooter>
@@ -3038,10 +3041,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3086,8 +3092,8 @@
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
       <c r="E4" s="122"/>
       <c r="G4" s="3"/>
       <c r="H4" s="7" t="s">
@@ -3102,9 +3108,9 @@
         <v>12</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="232"/>
       <c r="G5" s="3"/>
       <c r="H5" s="7" t="s">
         <v>13</v>
@@ -3126,83 +3132,83 @@
         <v>15</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="189"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
+      <c r="C7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
       <c r="G7" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="191"/>
-      <c r="I7" s="192"/>
-      <c r="J7" s="192"/>
-      <c r="K7" s="192"/>
+      <c r="H7" s="234"/>
+      <c r="I7" s="235"/>
+      <c r="J7" s="235"/>
+      <c r="K7" s="235"/>
     </row>
     <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="190"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="190"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
       <c r="G8" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="181"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="228"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="228"/>
     </row>
     <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="232"/>
       <c r="G9" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="181"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="182"/>
+      <c r="H9" s="227"/>
+      <c r="I9" s="228"/>
+      <c r="J9" s="228"/>
+      <c r="K9" s="228"/>
     </row>
     <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
       <c r="G10" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="181"/>
-      <c r="I10" s="182"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="182"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="228"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="228"/>
     </row>
     <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="181"/>
-      <c r="I11" s="182"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="182"/>
+      <c r="H11" s="227"/>
+      <c r="I11" s="228"/>
+      <c r="J11" s="228"/>
+      <c r="K11" s="228"/>
     </row>
     <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="G12" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="181"/>
-      <c r="I12" s="182"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="182"/>
+      <c r="H12" s="227"/>
+      <c r="I12" s="228"/>
+      <c r="J12" s="228"/>
+      <c r="K12" s="228"/>
     </row>
     <row r="13" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
@@ -3217,91 +3223,91 @@
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="48"/>
-      <c r="G14" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="197"/>
-      <c r="I14" s="198" t="s">
+      <c r="G14" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="225"/>
+      <c r="I14" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="199"/>
-      <c r="K14" s="200"/>
+      <c r="J14" s="198"/>
+      <c r="K14" s="199"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="251" t="s">
+      <c r="A15" s="236" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="264" t="s">
+      <c r="B15" s="239" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="264" t="s">
+      <c r="C15" s="239" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="264"/>
-      <c r="E15" s="256" t="s">
+      <c r="D15" s="239"/>
+      <c r="E15" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="266"/>
-      <c r="G15" s="208"/>
-      <c r="H15" s="209"/>
-      <c r="I15" s="210">
+      <c r="F15" s="242"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="206"/>
+      <c r="I15" s="207">
         <v>0.2</v>
       </c>
-      <c r="J15" s="213"/>
-      <c r="K15" s="215">
+      <c r="J15" s="210"/>
+      <c r="K15" s="212">
         <f>J15*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="263"/>
-      <c r="B16" s="264"/>
-      <c r="C16" s="264" t="s">
+      <c r="A16" s="237"/>
+      <c r="B16" s="239"/>
+      <c r="C16" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="264"/>
-      <c r="E16" s="267" t="s">
+      <c r="D16" s="239"/>
+      <c r="E16" s="243" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="268"/>
-      <c r="G16" s="219"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="211"/>
-      <c r="J16" s="213"/>
-      <c r="K16" s="215"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="190"/>
+      <c r="H16" s="191"/>
+      <c r="I16" s="208"/>
+      <c r="J16" s="210"/>
+      <c r="K16" s="212"/>
     </row>
     <row r="17" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="252"/>
-      <c r="B17" s="265"/>
-      <c r="C17" s="265" t="s">
+      <c r="A17" s="238"/>
+      <c r="B17" s="240"/>
+      <c r="C17" s="240" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="265"/>
-      <c r="E17" s="267" t="s">
+      <c r="D17" s="240"/>
+      <c r="E17" s="243" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="268"/>
-      <c r="G17" s="221"/>
-      <c r="H17" s="222"/>
-      <c r="I17" s="212"/>
-      <c r="J17" s="214"/>
-      <c r="K17" s="216"/>
+      <c r="F17" s="244"/>
+      <c r="G17" s="216"/>
+      <c r="H17" s="217"/>
+      <c r="I17" s="209"/>
+      <c r="J17" s="211"/>
+      <c r="K17" s="213"/>
     </row>
     <row r="18" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="251" t="s">
+      <c r="A18" s="236" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="253" t="s">
+      <c r="B18" s="260" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="254"/>
-      <c r="D18" s="255"/>
-      <c r="E18" s="256" t="s">
+      <c r="C18" s="261"/>
+      <c r="D18" s="262"/>
+      <c r="E18" s="241" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="257"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="220"/>
+      <c r="F18" s="263"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="191"/>
       <c r="I18" s="120">
         <v>0.4</v>
       </c>
@@ -3313,18 +3319,18 @@
       <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="252"/>
-      <c r="B19" s="258" t="s">
+      <c r="A19" s="238"/>
+      <c r="B19" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="259"/>
-      <c r="D19" s="260"/>
-      <c r="E19" s="261" t="s">
+      <c r="C19" s="265"/>
+      <c r="D19" s="266"/>
+      <c r="E19" s="267" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="262"/>
-      <c r="G19" s="219"/>
-      <c r="H19" s="220"/>
+      <c r="F19" s="268"/>
+      <c r="G19" s="190"/>
+      <c r="H19" s="191"/>
       <c r="I19" s="120">
         <v>0.4</v>
       </c>
@@ -3338,16 +3344,16 @@
       <c r="A20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="224"/>
-      <c r="D20" s="224"/>
-      <c r="E20" s="224"/>
-      <c r="F20" s="224"/>
-      <c r="G20" s="224"/>
-      <c r="H20" s="224"/>
-      <c r="I20" s="225"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="182"/>
       <c r="J20" s="121"/>
       <c r="K20" s="155"/>
     </row>
@@ -3487,7 +3493,7 @@
       <c r="F27" s="52"/>
       <c r="G27" s="1"/>
       <c r="H27" s="164">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I27" s="33" t="s">
         <v>86</v>
@@ -3511,88 +3517,88 @@
       <c r="K28" s="33"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="241" t="s">
+      <c r="A29" s="250" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="242"/>
-      <c r="C29" s="242"/>
-      <c r="D29" s="242"/>
-      <c r="E29" s="242"/>
-      <c r="F29" s="242"/>
-      <c r="G29" s="242"/>
-      <c r="H29" s="242"/>
-      <c r="I29" s="242"/>
-      <c r="J29" s="242"/>
-      <c r="K29" s="243"/>
+      <c r="B29" s="251"/>
+      <c r="C29" s="251"/>
+      <c r="D29" s="251"/>
+      <c r="E29" s="251"/>
+      <c r="F29" s="251"/>
+      <c r="G29" s="251"/>
+      <c r="H29" s="251"/>
+      <c r="I29" s="251"/>
+      <c r="J29" s="251"/>
+      <c r="K29" s="252"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="244"/>
-      <c r="B30" s="245"/>
-      <c r="C30" s="245"/>
-      <c r="D30" s="245"/>
-      <c r="E30" s="245"/>
-      <c r="F30" s="245"/>
-      <c r="G30" s="245"/>
-      <c r="H30" s="245"/>
-      <c r="I30" s="245"/>
-      <c r="J30" s="245"/>
-      <c r="K30" s="246"/>
+      <c r="A30" s="253"/>
+      <c r="B30" s="254"/>
+      <c r="C30" s="254"/>
+      <c r="D30" s="254"/>
+      <c r="E30" s="254"/>
+      <c r="F30" s="254"/>
+      <c r="G30" s="254"/>
+      <c r="H30" s="254"/>
+      <c r="I30" s="254"/>
+      <c r="J30" s="254"/>
+      <c r="K30" s="255"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="244"/>
-      <c r="B31" s="245"/>
-      <c r="C31" s="245"/>
-      <c r="D31" s="245"/>
-      <c r="E31" s="245"/>
-      <c r="F31" s="245"/>
-      <c r="G31" s="245"/>
-      <c r="H31" s="245"/>
-      <c r="I31" s="245"/>
-      <c r="J31" s="245"/>
-      <c r="K31" s="246"/>
+      <c r="A31" s="253"/>
+      <c r="B31" s="254"/>
+      <c r="C31" s="254"/>
+      <c r="D31" s="254"/>
+      <c r="E31" s="254"/>
+      <c r="F31" s="254"/>
+      <c r="G31" s="254"/>
+      <c r="H31" s="254"/>
+      <c r="I31" s="254"/>
+      <c r="J31" s="254"/>
+      <c r="K31" s="255"/>
     </row>
     <row r="32" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="244"/>
-      <c r="B32" s="245"/>
-      <c r="C32" s="245"/>
-      <c r="D32" s="245"/>
-      <c r="E32" s="245"/>
-      <c r="F32" s="245"/>
-      <c r="G32" s="245"/>
-      <c r="H32" s="245"/>
-      <c r="I32" s="245"/>
-      <c r="J32" s="245"/>
-      <c r="K32" s="246"/>
+      <c r="A32" s="253"/>
+      <c r="B32" s="254"/>
+      <c r="C32" s="254"/>
+      <c r="D32" s="254"/>
+      <c r="E32" s="254"/>
+      <c r="F32" s="254"/>
+      <c r="G32" s="254"/>
+      <c r="H32" s="254"/>
+      <c r="I32" s="254"/>
+      <c r="J32" s="254"/>
+      <c r="K32" s="255"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="247"/>
-      <c r="B33" s="248"/>
-      <c r="C33" s="248"/>
-      <c r="D33" s="248"/>
-      <c r="E33" s="248"/>
-      <c r="F33" s="248"/>
-      <c r="G33" s="248"/>
-      <c r="H33" s="248"/>
-      <c r="I33" s="248"/>
-      <c r="J33" s="248"/>
-      <c r="K33" s="249"/>
+      <c r="A33" s="256"/>
+      <c r="B33" s="257"/>
+      <c r="C33" s="257"/>
+      <c r="D33" s="257"/>
+      <c r="E33" s="257"/>
+      <c r="F33" s="257"/>
+      <c r="G33" s="257"/>
+      <c r="H33" s="257"/>
+      <c r="I33" s="257"/>
+      <c r="J33" s="257"/>
+      <c r="K33" s="258"/>
     </row>
     <row r="34" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="239" t="s">
+      <c r="A35" s="248" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="239"/>
-      <c r="C35" s="239"/>
-      <c r="D35" s="239"/>
-      <c r="E35" s="239"/>
-      <c r="F35" s="239"/>
-      <c r="G35" s="239"/>
-      <c r="H35" s="250">
+      <c r="B35" s="248"/>
+      <c r="C35" s="248"/>
+      <c r="D35" s="248"/>
+      <c r="E35" s="248"/>
+      <c r="F35" s="248"/>
+      <c r="G35" s="248"/>
+      <c r="H35" s="259">
         <f>K27</f>
         <v>0</v>
       </c>
-      <c r="I35" s="250"/>
+      <c r="I35" s="259"/>
       <c r="J35" s="34" t="s">
         <v>47</v>
       </c>
@@ -3602,20 +3608,20 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="239" t="s">
+      <c r="A36" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="239"/>
-      <c r="C36" s="239"/>
-      <c r="D36" s="239"/>
-      <c r="E36" s="239"/>
-      <c r="F36" s="239"/>
-      <c r="G36" s="239"/>
-      <c r="H36" s="240">
+      <c r="B36" s="248"/>
+      <c r="C36" s="248"/>
+      <c r="D36" s="248"/>
+      <c r="E36" s="248"/>
+      <c r="F36" s="248"/>
+      <c r="G36" s="248"/>
+      <c r="H36" s="249">
         <f>K21</f>
         <v>0</v>
       </c>
-      <c r="I36" s="240"/>
+      <c r="I36" s="249"/>
       <c r="J36" s="57" t="s">
         <v>63</v>
       </c>
@@ -3642,14 +3648,14 @@
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
       <c r="D38" s="52"/>
-      <c r="E38" s="236" t="s">
+      <c r="E38" s="245" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="237"/>
-      <c r="G38" s="237"/>
-      <c r="H38" s="237"/>
-      <c r="I38" s="237"/>
-      <c r="J38" s="238"/>
+      <c r="F38" s="246"/>
+      <c r="G38" s="246"/>
+      <c r="H38" s="246"/>
+      <c r="I38" s="246"/>
+      <c r="J38" s="247"/>
       <c r="K38" s="58">
         <f>K37/4</f>
         <v>0</v>
@@ -3733,32 +3739,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="A36:G36"/>
@@ -3775,6 +3755,32 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
   </mergeCells>
   <conditionalFormatting sqref="H36:I36 K15:K42">
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
@@ -3788,7 +3794,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LÄTTKLASS</oddHeader>
   </headerFooter>
@@ -3801,9 +3807,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
@@ -3852,9 +3861,9 @@
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
+      <c r="E4" s="233"/>
       <c r="F4" s="42"/>
       <c r="H4" s="3"/>
       <c r="I4" s="7" t="s">
@@ -3869,10 +3878,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
-      <c r="F5" s="189"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="232"/>
+      <c r="F5" s="232"/>
       <c r="H5" s="3"/>
       <c r="I5" s="7" t="s">
         <v>13</v>
@@ -3894,87 +3903,87 @@
         <v>15</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="189"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
-      <c r="F7" s="189"/>
+      <c r="C7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
+      <c r="F7" s="232"/>
       <c r="H7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="191"/>
-      <c r="J7" s="192"/>
-      <c r="K7" s="192"/>
-      <c r="L7" s="192"/>
+      <c r="I7" s="234"/>
+      <c r="J7" s="235"/>
+      <c r="K7" s="235"/>
+      <c r="L7" s="235"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="190"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="190"/>
-      <c r="F8" s="190"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
+      <c r="F8" s="233"/>
       <c r="H8" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="181"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
-      <c r="L8" s="182"/>
+      <c r="I8" s="227"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="228"/>
+      <c r="L8" s="228"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="189"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="232"/>
+      <c r="F9" s="232"/>
       <c r="H9" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="181"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="182"/>
-      <c r="L9" s="182"/>
+      <c r="I9" s="227"/>
+      <c r="J9" s="228"/>
+      <c r="K9" s="228"/>
+      <c r="L9" s="228"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
+      <c r="F10" s="232"/>
       <c r="H10" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="181"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="182"/>
-      <c r="L10" s="182"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="228"/>
+      <c r="L10" s="228"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="181"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="182"/>
-      <c r="L11" s="182"/>
+      <c r="I11" s="227"/>
+      <c r="J11" s="228"/>
+      <c r="K11" s="228"/>
+      <c r="L11" s="228"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="H12" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="181"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="182"/>
-      <c r="L12" s="182"/>
+      <c r="I12" s="227"/>
+      <c r="J12" s="228"/>
+      <c r="K12" s="228"/>
+      <c r="L12" s="228"/>
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
@@ -3990,95 +3999,95 @@
       <c r="E14" s="48"/>
       <c r="F14" s="48"/>
       <c r="G14" s="48"/>
-      <c r="H14" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="197"/>
-      <c r="J14" s="198" t="s">
+      <c r="H14" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="225"/>
+      <c r="J14" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="199"/>
-      <c r="L14" s="200"/>
+      <c r="K14" s="198"/>
+      <c r="L14" s="199"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="251" t="s">
+      <c r="A15" s="236" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="264" t="s">
+      <c r="B15" s="239" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="264" t="s">
+      <c r="C15" s="239" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="264"/>
-      <c r="E15" s="264"/>
-      <c r="F15" s="256" t="s">
+      <c r="D15" s="239"/>
+      <c r="E15" s="239"/>
+      <c r="F15" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="266"/>
-      <c r="H15" s="208"/>
-      <c r="I15" s="209"/>
-      <c r="J15" s="210">
+      <c r="G15" s="242"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="206"/>
+      <c r="J15" s="207">
         <v>0.2</v>
       </c>
-      <c r="K15" s="213"/>
-      <c r="L15" s="215">
+      <c r="K15" s="210"/>
+      <c r="L15" s="212">
         <f>K15*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="263"/>
-      <c r="B16" s="264"/>
-      <c r="C16" s="264" t="s">
+      <c r="A16" s="237"/>
+      <c r="B16" s="239"/>
+      <c r="C16" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="264"/>
-      <c r="E16" s="264"/>
-      <c r="F16" s="267" t="s">
+      <c r="D16" s="239"/>
+      <c r="E16" s="239"/>
+      <c r="F16" s="243" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="268"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="211"/>
-      <c r="K16" s="213"/>
-      <c r="L16" s="215"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="190"/>
+      <c r="I16" s="191"/>
+      <c r="J16" s="208"/>
+      <c r="K16" s="210"/>
+      <c r="L16" s="212"/>
     </row>
     <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="252"/>
-      <c r="B17" s="265"/>
-      <c r="C17" s="265" t="s">
+      <c r="A17" s="238"/>
+      <c r="B17" s="240"/>
+      <c r="C17" s="240" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="265"/>
-      <c r="E17" s="265"/>
-      <c r="F17" s="267" t="s">
+      <c r="D17" s="240"/>
+      <c r="E17" s="240"/>
+      <c r="F17" s="243" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="268"/>
-      <c r="H17" s="221"/>
-      <c r="I17" s="222"/>
-      <c r="J17" s="212"/>
-      <c r="K17" s="214"/>
-      <c r="L17" s="216"/>
+      <c r="G17" s="244"/>
+      <c r="H17" s="216"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="209"/>
+      <c r="K17" s="211"/>
+      <c r="L17" s="213"/>
     </row>
     <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="251" t="s">
+      <c r="A18" s="236" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="253" t="s">
+      <c r="B18" s="260" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="254"/>
-      <c r="D18" s="254"/>
-      <c r="E18" s="255"/>
-      <c r="F18" s="256" t="s">
+      <c r="C18" s="261"/>
+      <c r="D18" s="261"/>
+      <c r="E18" s="262"/>
+      <c r="F18" s="241" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="257"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="220"/>
+      <c r="G18" s="263"/>
+      <c r="H18" s="190"/>
+      <c r="I18" s="191"/>
       <c r="J18" s="49">
         <v>0.4</v>
       </c>
@@ -4090,19 +4099,19 @@
       <c r="M18" s="26"/>
     </row>
     <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="252"/>
-      <c r="B19" s="258" t="s">
+      <c r="A19" s="238"/>
+      <c r="B19" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="259"/>
-      <c r="D19" s="259"/>
-      <c r="E19" s="260"/>
-      <c r="F19" s="261" t="s">
+      <c r="C19" s="265"/>
+      <c r="D19" s="265"/>
+      <c r="E19" s="266"/>
+      <c r="F19" s="267" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="262"/>
-      <c r="H19" s="219"/>
-      <c r="I19" s="220"/>
+      <c r="G19" s="268"/>
+      <c r="H19" s="190"/>
+      <c r="I19" s="191"/>
       <c r="J19" s="49">
         <v>0.4</v>
       </c>
@@ -4116,17 +4125,17 @@
       <c r="A20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="223" t="s">
+      <c r="B20" s="180" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="224"/>
-      <c r="D20" s="224"/>
-      <c r="E20" s="224"/>
-      <c r="F20" s="224"/>
-      <c r="G20" s="224"/>
-      <c r="H20" s="224"/>
-      <c r="I20" s="224"/>
-      <c r="J20" s="225"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="182"/>
       <c r="K20" s="50"/>
       <c r="L20" s="155"/>
     </row>
@@ -4164,88 +4173,88 @@
       <c r="L22" s="33"/>
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="241" t="s">
+      <c r="A23" s="250" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="242"/>
-      <c r="C23" s="242"/>
-      <c r="D23" s="242"/>
-      <c r="E23" s="242"/>
-      <c r="F23" s="242"/>
-      <c r="G23" s="242"/>
-      <c r="H23" s="242"/>
-      <c r="I23" s="242"/>
-      <c r="J23" s="242"/>
-      <c r="K23" s="242"/>
-      <c r="L23" s="243"/>
+      <c r="B23" s="251"/>
+      <c r="C23" s="251"/>
+      <c r="D23" s="251"/>
+      <c r="E23" s="251"/>
+      <c r="F23" s="251"/>
+      <c r="G23" s="251"/>
+      <c r="H23" s="251"/>
+      <c r="I23" s="251"/>
+      <c r="J23" s="251"/>
+      <c r="K23" s="251"/>
+      <c r="L23" s="252"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="244"/>
-      <c r="B24" s="245"/>
-      <c r="C24" s="245"/>
-      <c r="D24" s="245"/>
-      <c r="E24" s="245"/>
-      <c r="F24" s="245"/>
-      <c r="G24" s="245"/>
-      <c r="H24" s="245"/>
-      <c r="I24" s="245"/>
-      <c r="J24" s="245"/>
-      <c r="K24" s="245"/>
-      <c r="L24" s="246"/>
+      <c r="A24" s="253"/>
+      <c r="B24" s="254"/>
+      <c r="C24" s="254"/>
+      <c r="D24" s="254"/>
+      <c r="E24" s="254"/>
+      <c r="F24" s="254"/>
+      <c r="G24" s="254"/>
+      <c r="H24" s="254"/>
+      <c r="I24" s="254"/>
+      <c r="J24" s="254"/>
+      <c r="K24" s="254"/>
+      <c r="L24" s="255"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="244"/>
-      <c r="B25" s="245"/>
-      <c r="C25" s="245"/>
-      <c r="D25" s="245"/>
-      <c r="E25" s="245"/>
-      <c r="F25" s="245"/>
-      <c r="G25" s="245"/>
-      <c r="H25" s="245"/>
-      <c r="I25" s="245"/>
-      <c r="J25" s="245"/>
-      <c r="K25" s="245"/>
-      <c r="L25" s="246"/>
+      <c r="A25" s="253"/>
+      <c r="B25" s="254"/>
+      <c r="C25" s="254"/>
+      <c r="D25" s="254"/>
+      <c r="E25" s="254"/>
+      <c r="F25" s="254"/>
+      <c r="G25" s="254"/>
+      <c r="H25" s="254"/>
+      <c r="I25" s="254"/>
+      <c r="J25" s="254"/>
+      <c r="K25" s="254"/>
+      <c r="L25" s="255"/>
     </row>
     <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="244"/>
-      <c r="B26" s="245"/>
-      <c r="C26" s="245"/>
-      <c r="D26" s="245"/>
-      <c r="E26" s="245"/>
-      <c r="F26" s="245"/>
-      <c r="G26" s="245"/>
-      <c r="H26" s="245"/>
-      <c r="I26" s="245"/>
-      <c r="J26" s="245"/>
-      <c r="K26" s="245"/>
-      <c r="L26" s="246"/>
+      <c r="A26" s="253"/>
+      <c r="B26" s="254"/>
+      <c r="C26" s="254"/>
+      <c r="D26" s="254"/>
+      <c r="E26" s="254"/>
+      <c r="F26" s="254"/>
+      <c r="G26" s="254"/>
+      <c r="H26" s="254"/>
+      <c r="I26" s="254"/>
+      <c r="J26" s="254"/>
+      <c r="K26" s="254"/>
+      <c r="L26" s="255"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="247"/>
-      <c r="B27" s="248"/>
-      <c r="C27" s="248"/>
-      <c r="D27" s="248"/>
-      <c r="E27" s="248"/>
-      <c r="F27" s="248"/>
-      <c r="G27" s="248"/>
-      <c r="H27" s="248"/>
-      <c r="I27" s="248"/>
-      <c r="J27" s="248"/>
-      <c r="K27" s="248"/>
-      <c r="L27" s="249"/>
+      <c r="A27" s="256"/>
+      <c r="B27" s="257"/>
+      <c r="C27" s="257"/>
+      <c r="D27" s="257"/>
+      <c r="E27" s="257"/>
+      <c r="F27" s="257"/>
+      <c r="G27" s="257"/>
+      <c r="H27" s="257"/>
+      <c r="I27" s="257"/>
+      <c r="J27" s="257"/>
+      <c r="K27" s="257"/>
+      <c r="L27" s="258"/>
     </row>
     <row r="29" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="239" t="s">
+      <c r="A29" s="248" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="239"/>
-      <c r="C29" s="239"/>
-      <c r="D29" s="239"/>
-      <c r="E29" s="239"/>
-      <c r="F29" s="239"/>
-      <c r="G29" s="239"/>
-      <c r="H29" s="239"/>
+      <c r="B29" s="248"/>
+      <c r="C29" s="248"/>
+      <c r="D29" s="248"/>
+      <c r="E29" s="248"/>
+      <c r="F29" s="248"/>
+      <c r="G29" s="248"/>
+      <c r="H29" s="248"/>
       <c r="I29" s="269"/>
       <c r="J29" s="269"/>
       <c r="K29" s="65" t="s">
@@ -4257,16 +4266,16 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="239" t="s">
+      <c r="A30" s="248" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="239"/>
-      <c r="C30" s="239"/>
-      <c r="D30" s="239"/>
-      <c r="E30" s="239"/>
-      <c r="F30" s="239"/>
-      <c r="G30" s="239"/>
-      <c r="H30" s="239"/>
+      <c r="B30" s="248"/>
+      <c r="C30" s="248"/>
+      <c r="D30" s="248"/>
+      <c r="E30" s="248"/>
+      <c r="F30" s="248"/>
+      <c r="G30" s="248"/>
+      <c r="H30" s="248"/>
       <c r="I30" s="269"/>
       <c r="J30" s="269"/>
       <c r="K30" s="45" t="s">
@@ -4278,16 +4287,16 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="239" t="s">
+      <c r="A31" s="248" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="239"/>
-      <c r="C31" s="239"/>
-      <c r="D31" s="239"/>
-      <c r="E31" s="239"/>
-      <c r="F31" s="239"/>
-      <c r="G31" s="239"/>
-      <c r="H31" s="239"/>
+      <c r="B31" s="248"/>
+      <c r="C31" s="248"/>
+      <c r="D31" s="248"/>
+      <c r="E31" s="248"/>
+      <c r="F31" s="248"/>
+      <c r="G31" s="248"/>
+      <c r="H31" s="248"/>
       <c r="I31" s="269"/>
       <c r="J31" s="269"/>
       <c r="K31" s="150" t="s">
@@ -4299,16 +4308,16 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="239" t="s">
+      <c r="A32" s="248" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="239"/>
-      <c r="C32" s="239"/>
-      <c r="D32" s="239"/>
-      <c r="E32" s="239"/>
-      <c r="F32" s="239"/>
-      <c r="G32" s="239"/>
-      <c r="H32" s="239"/>
+      <c r="B32" s="248"/>
+      <c r="C32" s="248"/>
+      <c r="D32" s="248"/>
+      <c r="E32" s="248"/>
+      <c r="F32" s="248"/>
+      <c r="G32" s="248"/>
+      <c r="H32" s="248"/>
       <c r="I32" s="269"/>
       <c r="J32" s="269"/>
       <c r="K32" s="45" t="s">
@@ -4320,21 +4329,21 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="239" t="s">
+      <c r="A33" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="239"/>
-      <c r="C33" s="239"/>
-      <c r="D33" s="239"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="239"/>
-      <c r="G33" s="239"/>
-      <c r="H33" s="239"/>
-      <c r="I33" s="240">
+      <c r="B33" s="248"/>
+      <c r="C33" s="248"/>
+      <c r="D33" s="248"/>
+      <c r="E33" s="248"/>
+      <c r="F33" s="248"/>
+      <c r="G33" s="248"/>
+      <c r="H33" s="248"/>
+      <c r="I33" s="249">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="J33" s="240"/>
+      <c r="J33" s="249"/>
       <c r="K33" s="150" t="s">
         <v>110</v>
       </c>
@@ -4362,14 +4371,14 @@
       <c r="C35" s="52"/>
       <c r="D35" s="52"/>
       <c r="E35" s="52"/>
-      <c r="F35" s="236" t="s">
+      <c r="F35" s="245" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="237"/>
-      <c r="H35" s="237"/>
-      <c r="I35" s="237"/>
-      <c r="J35" s="237"/>
-      <c r="K35" s="238"/>
+      <c r="G35" s="246"/>
+      <c r="H35" s="246"/>
+      <c r="I35" s="246"/>
+      <c r="J35" s="246"/>
+      <c r="K35" s="247"/>
       <c r="L35" s="58">
         <f>L34/10</f>
         <v>0</v>
@@ -4480,26 +4489,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="A15:A17"/>
@@ -4516,18 +4517,26 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <conditionalFormatting sqref="L15:L39 I33:J33">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
@@ -4541,7 +4550,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LÄTTKLASS</oddHeader>
   </headerFooter>
@@ -4554,10 +4563,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -4605,9 +4617,9 @@
         <v>10</v>
       </c>
       <c r="B4" s="75"/>
-      <c r="C4" s="270"/>
-      <c r="D4" s="270"/>
-      <c r="E4" s="270"/>
+      <c r="C4" s="273"/>
+      <c r="D4" s="273"/>
+      <c r="E4" s="273"/>
       <c r="F4" s="104"/>
       <c r="H4" s="102"/>
       <c r="I4" s="101" t="s">
@@ -4667,10 +4679,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="75"/>
-      <c r="C8" s="270"/>
-      <c r="D8" s="270"/>
-      <c r="E8" s="270"/>
-      <c r="F8" s="270"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
       <c r="H8" s="94"/>
       <c r="I8" s="94"/>
       <c r="J8" s="94"/>
@@ -4874,96 +4886,96 @@
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
-      <c r="G23" s="271" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="272"/>
-      <c r="I23" s="273"/>
-      <c r="J23" s="198" t="s">
+      <c r="G23" s="274" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="275"/>
+      <c r="I23" s="276"/>
+      <c r="J23" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="199"/>
-      <c r="L23" s="200"/>
+      <c r="K23" s="198"/>
+      <c r="L23" s="199"/>
     </row>
     <row r="24" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="201" t="s">
+      <c r="A24" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="204" t="s">
+      <c r="B24" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="204" t="s">
+      <c r="C24" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="204"/>
-      <c r="E24" s="206" t="s">
+      <c r="D24" s="201"/>
+      <c r="E24" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="283"/>
-      <c r="G24" s="274"/>
-      <c r="H24" s="275"/>
-      <c r="I24" s="276"/>
-      <c r="J24" s="210">
+      <c r="F24" s="270"/>
+      <c r="G24" s="277"/>
+      <c r="H24" s="278"/>
+      <c r="I24" s="279"/>
+      <c r="J24" s="207">
         <v>0.2</v>
       </c>
-      <c r="K24" s="213"/>
-      <c r="L24" s="216">
+      <c r="K24" s="210"/>
+      <c r="L24" s="213">
         <f>K24*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="202"/>
-      <c r="B25" s="204"/>
-      <c r="C25" s="204" t="s">
+      <c r="A25" s="200"/>
+      <c r="B25" s="201"/>
+      <c r="C25" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="204"/>
-      <c r="E25" s="217" t="s">
+      <c r="D25" s="201"/>
+      <c r="E25" s="214" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="218"/>
-      <c r="G25" s="277"/>
-      <c r="H25" s="278"/>
-      <c r="I25" s="279"/>
-      <c r="J25" s="211"/>
-      <c r="K25" s="213"/>
-      <c r="L25" s="284"/>
+      <c r="F25" s="215"/>
+      <c r="G25" s="280"/>
+      <c r="H25" s="281"/>
+      <c r="I25" s="282"/>
+      <c r="J25" s="208"/>
+      <c r="K25" s="210"/>
+      <c r="L25" s="271"/>
     </row>
     <row r="26" spans="1:13" s="11" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="203"/>
-      <c r="B26" s="205"/>
-      <c r="C26" s="205" t="s">
+      <c r="A26" s="184"/>
+      <c r="B26" s="202"/>
+      <c r="C26" s="202" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="205"/>
-      <c r="E26" s="217" t="s">
+      <c r="D26" s="202"/>
+      <c r="E26" s="214" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="218"/>
-      <c r="G26" s="277"/>
-      <c r="H26" s="278"/>
-      <c r="I26" s="279"/>
-      <c r="J26" s="212"/>
-      <c r="K26" s="214"/>
-      <c r="L26" s="285"/>
+      <c r="F26" s="215"/>
+      <c r="G26" s="280"/>
+      <c r="H26" s="281"/>
+      <c r="I26" s="282"/>
+      <c r="J26" s="209"/>
+      <c r="K26" s="211"/>
+      <c r="L26" s="272"/>
     </row>
     <row r="27" spans="1:13" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="201" t="s">
+      <c r="A27" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="226" t="s">
+      <c r="B27" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="227"/>
-      <c r="D27" s="228"/>
-      <c r="E27" s="229" t="s">
+      <c r="C27" s="186"/>
+      <c r="D27" s="187"/>
+      <c r="E27" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="230"/>
-      <c r="G27" s="280"/>
-      <c r="H27" s="281"/>
-      <c r="I27" s="282"/>
+      <c r="F27" s="189"/>
+      <c r="G27" s="283"/>
+      <c r="H27" s="284"/>
+      <c r="I27" s="285"/>
       <c r="J27" s="66">
         <v>0.4</v>
       </c>
@@ -4975,19 +4987,19 @@
       <c r="M27" s="26"/>
     </row>
     <row r="28" spans="1:13" s="11" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="203"/>
-      <c r="B28" s="231" t="s">
+      <c r="A28" s="184"/>
+      <c r="B28" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="232"/>
-      <c r="D28" s="233"/>
-      <c r="E28" s="234" t="s">
+      <c r="C28" s="193"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="195" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="235"/>
-      <c r="G28" s="277"/>
-      <c r="H28" s="278"/>
-      <c r="I28" s="279"/>
+      <c r="F28" s="196"/>
+      <c r="G28" s="280"/>
+      <c r="H28" s="281"/>
+      <c r="I28" s="282"/>
       <c r="J28" s="66">
         <v>0.4</v>
       </c>
@@ -5001,16 +5013,16 @@
       <c r="A29" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="223" t="s">
+      <c r="B29" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="224"/>
-      <c r="D29" s="224"/>
-      <c r="E29" s="224"/>
-      <c r="F29" s="224"/>
-      <c r="G29" s="224"/>
-      <c r="H29" s="224"/>
-      <c r="I29" s="225"/>
+      <c r="C29" s="181"/>
+      <c r="D29" s="181"/>
+      <c r="E29" s="181"/>
+      <c r="F29" s="181"/>
+      <c r="G29" s="181"/>
+      <c r="H29" s="181"/>
+      <c r="I29" s="182"/>
       <c r="J29" s="67"/>
       <c r="K29" s="61">
         <f>J29</f>
@@ -5127,23 +5139,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:F28"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="B29:I29"/>
     <mergeCell ref="G23:I23"/>
@@ -5157,6 +5152,23 @@
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="L24 L27:L28 K29 L30:L32">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
@@ -5170,7 +5182,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LÄTTKLASS</oddHeader>
   </headerFooter>
@@ -5180,9 +5192,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -5232,9 +5247,9 @@
         <v>10</v>
       </c>
       <c r="B4" s="111"/>
-      <c r="C4" s="287"/>
-      <c r="D4" s="287"/>
-      <c r="E4" s="287"/>
+      <c r="C4" s="294"/>
+      <c r="D4" s="294"/>
+      <c r="E4" s="294"/>
       <c r="F4" s="118"/>
       <c r="H4" s="79" t="s">
         <v>11</v>
@@ -5249,10 +5264,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="115"/>
-      <c r="C5" s="288"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="288"/>
-      <c r="F5" s="288"/>
+      <c r="C5" s="293"/>
+      <c r="D5" s="293"/>
+      <c r="E5" s="293"/>
+      <c r="F5" s="293"/>
       <c r="H5" s="79" t="s">
         <v>13</v>
       </c>
@@ -5266,10 +5281,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="115"/>
-      <c r="C6" s="288"/>
-      <c r="D6" s="288"/>
-      <c r="E6" s="288"/>
-      <c r="F6" s="288"/>
+      <c r="C6" s="293"/>
+      <c r="D6" s="293"/>
+      <c r="E6" s="293"/>
+      <c r="F6" s="293"/>
       <c r="H6" s="68"/>
       <c r="I6" s="68"/>
       <c r="J6" s="68"/>
@@ -5298,10 +5313,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="111"/>
-      <c r="C8" s="287"/>
-      <c r="D8" s="287"/>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
+      <c r="C8" s="294"/>
+      <c r="D8" s="294"/>
+      <c r="E8" s="294"/>
+      <c r="F8" s="294"/>
       <c r="H8" s="117"/>
       <c r="I8" s="117"/>
       <c r="J8" s="117"/>
@@ -5313,10 +5328,10 @@
         <v>19</v>
       </c>
       <c r="B9" s="115"/>
-      <c r="C9" s="288"/>
-      <c r="D9" s="288"/>
-      <c r="E9" s="288"/>
-      <c r="F9" s="288"/>
+      <c r="C9" s="293"/>
+      <c r="D9" s="293"/>
+      <c r="E9" s="293"/>
+      <c r="F9" s="293"/>
       <c r="H9" s="117"/>
       <c r="I9" s="117"/>
       <c r="J9" s="117"/>
@@ -5328,10 +5343,10 @@
         <v>30</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="288"/>
-      <c r="D10" s="288"/>
-      <c r="E10" s="288"/>
-      <c r="F10" s="288"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
       <c r="H10" s="117"/>
       <c r="I10" s="117"/>
       <c r="J10" s="117"/>
@@ -5368,93 +5383,93 @@
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="48"/>
-      <c r="G13" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="197"/>
-      <c r="I13" s="198" t="s">
+      <c r="G13" s="224" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="225"/>
+      <c r="I13" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="199"/>
-      <c r="K13" s="200"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="199"/>
     </row>
     <row r="14" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="251" t="s">
+      <c r="A14" s="236" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="264" t="s">
+      <c r="B14" s="239" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="264" t="s">
+      <c r="C14" s="239" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="264"/>
-      <c r="E14" s="256" t="s">
+      <c r="D14" s="239"/>
+      <c r="E14" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="266"/>
-      <c r="G14" s="208"/>
-      <c r="H14" s="209"/>
-      <c r="I14" s="210">
+      <c r="F14" s="242"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="206"/>
+      <c r="I14" s="207">
         <v>0.2</v>
       </c>
-      <c r="J14" s="213">
-        <v>0</v>
-      </c>
-      <c r="K14" s="215">
+      <c r="J14" s="210">
+        <v>0</v>
+      </c>
+      <c r="K14" s="212">
         <f>J14*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="263"/>
-      <c r="B15" s="264"/>
-      <c r="C15" s="264" t="s">
+      <c r="A15" s="237"/>
+      <c r="B15" s="239"/>
+      <c r="C15" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="264"/>
-      <c r="E15" s="267" t="s">
+      <c r="D15" s="239"/>
+      <c r="E15" s="243" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="268"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="211"/>
-      <c r="J15" s="213"/>
-      <c r="K15" s="215"/>
+      <c r="F15" s="244"/>
+      <c r="G15" s="190"/>
+      <c r="H15" s="191"/>
+      <c r="I15" s="208"/>
+      <c r="J15" s="210"/>
+      <c r="K15" s="212"/>
     </row>
     <row r="16" spans="1:12" s="11" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="252"/>
-      <c r="B16" s="265"/>
-      <c r="C16" s="265" t="s">
+      <c r="A16" s="238"/>
+      <c r="B16" s="240"/>
+      <c r="C16" s="240" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="265"/>
-      <c r="E16" s="267" t="s">
+      <c r="D16" s="240"/>
+      <c r="E16" s="243" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="268"/>
-      <c r="G16" s="221"/>
-      <c r="H16" s="222"/>
-      <c r="I16" s="212"/>
-      <c r="J16" s="214"/>
-      <c r="K16" s="216"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="216"/>
+      <c r="H16" s="217"/>
+      <c r="I16" s="209"/>
+      <c r="J16" s="211"/>
+      <c r="K16" s="213"/>
     </row>
     <row r="17" spans="1:12" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="251" t="s">
+      <c r="A17" s="236" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="253" t="s">
+      <c r="B17" s="260" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="254"/>
-      <c r="D17" s="255"/>
-      <c r="E17" s="256" t="s">
+      <c r="C17" s="261"/>
+      <c r="D17" s="262"/>
+      <c r="E17" s="241" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="257"/>
-      <c r="G17" s="219"/>
-      <c r="H17" s="220"/>
+      <c r="F17" s="263"/>
+      <c r="G17" s="190"/>
+      <c r="H17" s="191"/>
       <c r="I17" s="49">
         <v>0.4</v>
       </c>
@@ -5468,18 +5483,18 @@
       <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" s="11" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="252"/>
-      <c r="B18" s="258" t="s">
+      <c r="A18" s="238"/>
+      <c r="B18" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="259"/>
-      <c r="D18" s="260"/>
-      <c r="E18" s="261" t="s">
+      <c r="C18" s="265"/>
+      <c r="D18" s="266"/>
+      <c r="E18" s="267" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="262"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="220"/>
+      <c r="F18" s="268"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="191"/>
       <c r="I18" s="49">
         <v>0.4</v>
       </c>
@@ -5495,16 +5510,16 @@
       <c r="A19" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="223" t="s">
+      <c r="B19" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="224"/>
-      <c r="D19" s="224"/>
-      <c r="E19" s="224"/>
-      <c r="F19" s="224"/>
-      <c r="G19" s="224"/>
-      <c r="H19" s="224"/>
-      <c r="I19" s="225"/>
+      <c r="C19" s="181"/>
+      <c r="D19" s="181"/>
+      <c r="E19" s="181"/>
+      <c r="F19" s="181"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="181"/>
+      <c r="I19" s="182"/>
       <c r="J19" s="50"/>
       <c r="K19" s="155"/>
     </row>
@@ -5624,88 +5639,88 @@
       <c r="K25" s="33"/>
     </row>
     <row r="26" spans="1:12" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="241" t="s">
+      <c r="A26" s="250" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="242"/>
-      <c r="C26" s="242"/>
-      <c r="D26" s="242"/>
-      <c r="E26" s="242"/>
-      <c r="F26" s="242"/>
-      <c r="G26" s="242"/>
-      <c r="H26" s="242"/>
-      <c r="I26" s="242"/>
-      <c r="J26" s="242"/>
-      <c r="K26" s="243"/>
+      <c r="B26" s="251"/>
+      <c r="C26" s="251"/>
+      <c r="D26" s="251"/>
+      <c r="E26" s="251"/>
+      <c r="F26" s="251"/>
+      <c r="G26" s="251"/>
+      <c r="H26" s="251"/>
+      <c r="I26" s="251"/>
+      <c r="J26" s="251"/>
+      <c r="K26" s="252"/>
     </row>
     <row r="27" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="244"/>
-      <c r="B27" s="245"/>
-      <c r="C27" s="245"/>
-      <c r="D27" s="245"/>
-      <c r="E27" s="245"/>
-      <c r="F27" s="245"/>
-      <c r="G27" s="245"/>
-      <c r="H27" s="245"/>
-      <c r="I27" s="245"/>
-      <c r="J27" s="245"/>
-      <c r="K27" s="246"/>
+      <c r="A27" s="253"/>
+      <c r="B27" s="254"/>
+      <c r="C27" s="254"/>
+      <c r="D27" s="254"/>
+      <c r="E27" s="254"/>
+      <c r="F27" s="254"/>
+      <c r="G27" s="254"/>
+      <c r="H27" s="254"/>
+      <c r="I27" s="254"/>
+      <c r="J27" s="254"/>
+      <c r="K27" s="255"/>
     </row>
     <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="244"/>
-      <c r="B28" s="245"/>
-      <c r="C28" s="245"/>
-      <c r="D28" s="245"/>
-      <c r="E28" s="245"/>
-      <c r="F28" s="245"/>
-      <c r="G28" s="245"/>
-      <c r="H28" s="245"/>
-      <c r="I28" s="245"/>
-      <c r="J28" s="245"/>
-      <c r="K28" s="246"/>
+      <c r="A28" s="253"/>
+      <c r="B28" s="254"/>
+      <c r="C28" s="254"/>
+      <c r="D28" s="254"/>
+      <c r="E28" s="254"/>
+      <c r="F28" s="254"/>
+      <c r="G28" s="254"/>
+      <c r="H28" s="254"/>
+      <c r="I28" s="254"/>
+      <c r="J28" s="254"/>
+      <c r="K28" s="255"/>
     </row>
     <row r="29" spans="1:12" s="11" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="244"/>
-      <c r="B29" s="245"/>
-      <c r="C29" s="245"/>
-      <c r="D29" s="245"/>
-      <c r="E29" s="245"/>
-      <c r="F29" s="245"/>
-      <c r="G29" s="245"/>
-      <c r="H29" s="245"/>
-      <c r="I29" s="245"/>
-      <c r="J29" s="245"/>
-      <c r="K29" s="246"/>
+      <c r="A29" s="253"/>
+      <c r="B29" s="254"/>
+      <c r="C29" s="254"/>
+      <c r="D29" s="254"/>
+      <c r="E29" s="254"/>
+      <c r="F29" s="254"/>
+      <c r="G29" s="254"/>
+      <c r="H29" s="254"/>
+      <c r="I29" s="254"/>
+      <c r="J29" s="254"/>
+      <c r="K29" s="255"/>
     </row>
     <row r="30" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="247"/>
-      <c r="B30" s="248"/>
-      <c r="C30" s="248"/>
-      <c r="D30" s="248"/>
-      <c r="E30" s="248"/>
-      <c r="F30" s="248"/>
-      <c r="G30" s="248"/>
-      <c r="H30" s="248"/>
-      <c r="I30" s="248"/>
-      <c r="J30" s="248"/>
-      <c r="K30" s="249"/>
+      <c r="A30" s="256"/>
+      <c r="B30" s="257"/>
+      <c r="C30" s="257"/>
+      <c r="D30" s="257"/>
+      <c r="E30" s="257"/>
+      <c r="F30" s="257"/>
+      <c r="G30" s="257"/>
+      <c r="H30" s="257"/>
+      <c r="I30" s="257"/>
+      <c r="J30" s="257"/>
+      <c r="K30" s="258"/>
     </row>
     <row r="31" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="292" t="s">
+      <c r="A32" s="290" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="292"/>
-      <c r="C32" s="292"/>
-      <c r="D32" s="292"/>
-      <c r="E32" s="292"/>
-      <c r="F32" s="292"/>
-      <c r="G32" s="292"/>
-      <c r="H32" s="294">
+      <c r="B32" s="290"/>
+      <c r="C32" s="290"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="292">
         <f>G24</f>
         <v>0</v>
       </c>
-      <c r="I32" s="294"/>
+      <c r="I32" s="292"/>
       <c r="J32" s="165" t="s">
         <v>47</v>
       </c>
@@ -5715,20 +5730,20 @@
       </c>
     </row>
     <row r="33" spans="1:12" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="292" t="s">
+      <c r="A33" s="290" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="292"/>
-      <c r="C33" s="292"/>
-      <c r="D33" s="292"/>
-      <c r="E33" s="292"/>
-      <c r="F33" s="292"/>
-      <c r="G33" s="292"/>
-      <c r="H33" s="250">
+      <c r="B33" s="290"/>
+      <c r="C33" s="290"/>
+      <c r="D33" s="290"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="259">
         <f>K20</f>
         <v>0</v>
       </c>
-      <c r="I33" s="293"/>
+      <c r="I33" s="291"/>
       <c r="J33" s="166" t="s">
         <v>63</v>
       </c>
@@ -5760,14 +5775,14 @@
       <c r="B35" s="167"/>
       <c r="C35" s="167"/>
       <c r="D35" s="167"/>
-      <c r="E35" s="289" t="s">
+      <c r="E35" s="287" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="290"/>
-      <c r="G35" s="290"/>
-      <c r="H35" s="290"/>
-      <c r="I35" s="290"/>
-      <c r="J35" s="291"/>
+      <c r="F35" s="288"/>
+      <c r="G35" s="288"/>
+      <c r="H35" s="288"/>
+      <c r="I35" s="288"/>
+      <c r="J35" s="289"/>
       <c r="K35" s="58">
         <f>K34/4</f>
         <v>0</v>
@@ -5858,26 +5873,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="A26:K30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="I13:K13"/>
@@ -5894,6 +5889,26 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="A26:K30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="H32:I32"/>
   </mergeCells>
   <conditionalFormatting sqref="H33:I33 K14:K21 J22:J24 K25:K40">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
@@ -5907,7 +5922,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LÄTTKLASS</oddHeader>
   </headerFooter>

</xml_diff>